<commit_message>
Adding additional comments to cases with multiple ss_ids, about the dois of these ss_ids: are they the same? are the dois missing? are the dois different?
</commit_message>
<xml_diff>
--- a/scripts/script_data/TEMP_LOOKUP_matches_single_bibkey_with_none_one_or_many_ss_ids.xlsx
+++ b/scripts/script_data/TEMP_LOOKUP_matches_single_bibkey_with_none_one_or_many_ss_ids.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I120"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,7 +542,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['69999230b02054b82254684a73bb8a4c83878d28', 'b4c4c3dc91d42114023b0575c3e2273b87446ff7']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['69999230b02054b82254684a73bb8a4c83878d28', 'b4c4c3dc91d42114023b0575c3e2273b87446ff7']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -616,7 +616,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>multiple doi matches ['979a9f247700d00ff2c3f0612d5eb001379f93c8', 'c397c6f1480ac8e3ed875adad96e9b3e00c37f26'], took the first one with most citations</t>
+          <t>[ss_ids: same DOI] multiple doi matches ['979a9f247700d00ff2c3f0612d5eb001379f93c8', 'c397c6f1480ac8e3ed875adad96e9b3e00c37f26'], took the first one with most citations</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -690,7 +690,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['6425e3f4c37f8deb9e8dc933e34d49aa843635b9', 'cc7605f2b7e61723f12839fabc1066da0cc8744b']), took the first one with most citations</t>
+          <t>[ss_ids: no DOIs!] title matching: single bibkey with multiple_ss_ids (['6425e3f4c37f8deb9e8dc933e34d49aa843635b9', 'cc7605f2b7e61723f12839fabc1066da0cc8744b']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -733,7 +733,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['91bcebba717670d740ef76097a0885a0bd3c9dde', '94962ef85aca6df5c8289874b56bcaa8722dc596']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['91bcebba717670d740ef76097a0885a0bd3c9dde', '94962ef85aca6df5c8289874b56bcaa8722dc596']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['20fe29e553477d9bd330f052e4d01c0c1c616b22', 'f131ef217543d179269018950bf3b6ba2b30f3b1']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['20fe29e553477d9bd330f052e4d01c0c1c616b22', 'f131ef217543d179269018950bf3b6ba2b30f3b1']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -819,7 +819,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['4bcd672218ecec70473c84f6f1cc52c64031f3e5', 'bc6b483f9b1fa630fa4b43158b13716f1ca7497b']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['4bcd672218ecec70473c84f6f1cc52c64031f3e5', 'bc6b483f9b1fa630fa4b43158b13716f1ca7497b']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['aff9f3cd8024fb64c7ea36d396a36ebf33d01f5b', 'c3e98e4b01c27affe1b6c161172c5e27e8141618']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['aff9f3cd8024fb64c7ea36d396a36ebf33d01f5b', 'c3e98e4b01c27affe1b6c161172c5e27e8141618']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -936,7 +936,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['b0cc9473a96dcd45dd1c7de2d7d217c2a453a850', 'd5b8fba71671814445de80d36a2d563f43eb9d07']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['b0cc9473a96dcd45dd1c7de2d7d217c2a453a850', 'd5b8fba71671814445de80d36a2d563f43eb9d07']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['3ed451d2830a2afcbbd254f0015eeafa796ba1b7', '4fd1ad386d794e9baff286b212013b3b44bb7bd3']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['3ed451d2830a2afcbbd254f0015eeafa796ba1b7', '4fd1ad386d794e9baff286b212013b3b44bb7bd3']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['27cebb08aca785444166209593fc0ec740469b1b', '96438076b4dfa87956f55c0d8cef9c198de2beb7']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['27cebb08aca785444166209593fc0ec740469b1b', '96438076b4dfa87956f55c0d8cef9c198de2beb7']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['86b9d39fb026746752f95f87f87fd26b8512c913', 'fd0901b1f2121506391a7859de8fb695d159a393']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['86b9d39fb026746752f95f87f87fd26b8512c913', 'fd0901b1f2121506391a7859de8fb695d159a393']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['fb1084b454e9b6f203c860e6f89ca4389cd1a8e9', 'fc7b70a4d154e3d2dfabe4393809dfb29cc36a7a']), took the first one with most citations</t>
+          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['fb1084b454e9b6f203c860e6f89ca4389cd1a8e9', 'fc7b70a4d154e3d2dfabe4393809dfb29cc36a7a']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['d1e0a041fc417d82c584191ecf5b3b536127d9e0', 'e15e0cd21632aa9d6643b314a4d1d1a6580f2b39']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['d1e0a041fc417d82c584191ecf5b3b536127d9e0', 'e15e0cd21632aa9d6643b314a4d1d1a6580f2b39']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['2d7797e69a35b5ffe021a2762ef251764562dca4', 'c7ce6b90707871b922aca4cb6a8b16625980788b']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['2d7797e69a35b5ffe021a2762ef251764562dca4', 'c7ce6b90707871b922aca4cb6a8b16625980788b']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -1454,7 +1454,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['91feb0cb04d67a5c38d0a4e7c67fc7874491abc6', '925024223075dcc5b4db81f4b07eddf2cbdf4519']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['91feb0cb04d67a5c38d0a4e7c67fc7874491abc6', '925024223075dcc5b4db81f4b07eddf2cbdf4519']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['46479bbea7749cb2db35b139206039531327053c', 'b69fe5a837277ddbea5215d6bacd3a902e9d11ce']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['46479bbea7749cb2db35b139206039531327053c', 'b69fe5a837277ddbea5215d6bacd3a902e9d11ce']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['11cfab281e93fa7803931be8b589aa1f09d7af02', '8c4fab5306f4c4e179cfae2acd3427fb5d661627']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['11cfab281e93fa7803931be8b589aa1f09d7af02', '8c4fab5306f4c4e179cfae2acd3427fb5d661627']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['13122b7c0ef4a596875eff981651d60140e67417', '142f9f46a9ca5a99de4c7b819d801d245a9334ba']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['13122b7c0ef4a596875eff981651d60140e67417', '142f9f46a9ca5a99de4c7b819d801d245a9334ba']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['560e2100afbc64953c5155459b1f459f6e55003e', '65e6296fe63fbf76519ef01e16b5e62bfabbc3ca']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['560e2100afbc64953c5155459b1f459f6e55003e', '65e6296fe63fbf76519ef01e16b5e62bfabbc3ca']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['3881ae992914cd50a14782104170cc5dd5d9ae7e', 'a4d4e42f1accfd77f378549c776b7c850afbcda5']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['3881ae992914cd50a14782104170cc5dd5d9ae7e', 'a4d4e42f1accfd77f378549c776b7c850afbcda5']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['16352b9da95fb7a2643f617b61c56669b07879c8', '817c6ab7fde2a45210b6b80c4713b9147b3eba19']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['16352b9da95fb7a2643f617b61c56669b07879c8', '817c6ab7fde2a45210b6b80c4713b9147b3eba19']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['5e3b8647dd6da802cd06a3e8f193d4b2f2823410', 'a908e3775fd064b0d249728a7261cfb1efa13b87']), took the first one with most citations</t>
+          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['5e3b8647dd6da802cd06a3e8f193d4b2f2823410', 'a908e3775fd064b0d249728a7261cfb1efa13b87']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -2108,7 +2108,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['7c83ece3400fa10da80bd363c15dd96eded51c9f', '88b86ad75e10c7dac7b70edbd05ed494d699ffb0']), took the first one with most citations</t>
+          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['7c83ece3400fa10da80bd363c15dd96eded51c9f', '88b86ad75e10c7dac7b70edbd05ed494d699ffb0']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['889cc0565d6e2e844f4db0132c71a612672d2497', 'a7f96553bc690f6f66697895a98e9377cc0f7562']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['889cc0565d6e2e844f4db0132c71a612672d2497', 'a7f96553bc690f6f66697895a98e9377cc0f7562']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -2380,7 +2380,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['8678f63d7a648eb4d0f64e50c8ff5a1c53ac128b', '91d23b702b9a59bf75c5162c3250017b526c0e69', 'bed661aebb0ede3c407e044637ce60a6d7ccfe5f', 'fa96430855d805c045335e70c0b60d3acb8c9a79']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['8678f63d7a648eb4d0f64e50c8ff5a1c53ac128b', '91d23b702b9a59bf75c5162c3250017b526c0e69', 'bed661aebb0ede3c407e044637ce60a6d7ccfe5f', 'fa96430855d805c045335e70c0b60d3acb8c9a79']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['682e8febc5d053766fefe1ee2de5ca2ff39762f2', '7f1eabb6591699816ccd89e7765a66dc54a7175c', '86bab119f07a492350c6cc7bd06ed91c73ee807a', 'e7f15929ff71a5a33af66ece92d707a7be7aebc8']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['682e8febc5d053766fefe1ee2de5ca2ff39762f2', '7f1eabb6591699816ccd89e7765a66dc54a7175c', '86bab119f07a492350c6cc7bd06ed91c73ee807a', 'e7f15929ff71a5a33af66ece92d707a7be7aebc8']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -2559,7 +2559,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['6119971f513cfa3a9dce2cff139f041f11bcb404', 'fb5c4bf41fd879c9c64028a817db7f7ab6aba429']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['6119971f513cfa3a9dce2cff139f041f11bcb404', 'fb5c4bf41fd879c9c64028a817db7f7ab6aba429']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['6d37b7ceb99c6cc36be602ae9ab2a26232d11bb5', '8f938d6b54c38e469997969380383de635e654aa']), took the first one with most citations</t>
+          <t>[ss_ids: no DOIs!] title matching: single bibkey with multiple_ss_ids (['6d37b7ceb99c6cc36be602ae9ab2a26232d11bb5', '8f938d6b54c38e469997969380383de635e654aa']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -2800,7 +2800,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['18d0a58647fbdaaf7cd278cb66ae548a1e5289e5', '981fb8239e2e32cd742059aa270015871aa64b61']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['18d0a58647fbdaaf7cd278cb66ae548a1e5289e5', '981fb8239e2e32cd742059aa270015871aa64b61']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -2905,7 +2905,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>multiple doi matches ['0807697ee497d294c1ec272631c5f84aeeb2571e', 'c70d5169b5c69171cc2ed3ec40eebda0630988d9'], took the first one with most citations</t>
+          <t>[ss_ids: same DOI] multiple doi matches ['0807697ee497d294c1ec272631c5f84aeeb2571e', 'c70d5169b5c69171cc2ed3ec40eebda0630988d9'], took the first one with most citations</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -2979,7 +2979,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['6257ee97417d8bead217991caf7c3cd5b439e040', '787ef2981e94e481432cb2a1296903676ec80fa9']), took the first one with most citations</t>
+          <t>[ss_ids: no DOIs!] title matching: single bibkey with multiple_ss_ids (['6257ee97417d8bead217991caf7c3cd5b439e040', '787ef2981e94e481432cb2a1296903676ec80fa9']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -3022,7 +3022,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['75bc9847c96d8f319f82d1b9ba01b5a396247152', 'a6a2fed1ee525c0d2a35ae6454660eca53ce03fc', 'fdf663cc9dda29d55f2e2f44f9876f3b08f854f8']), took the first one with most citations</t>
+          <t>[ss_ids: 2 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['75bc9847c96d8f319f82d1b9ba01b5a396247152', 'a6a2fed1ee525c0d2a35ae6454660eca53ce03fc', 'fdf663cc9dda29d55f2e2f44f9876f3b08f854f8']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -3251,7 +3251,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['2fa5f435f41242e8ef053e94ae7af400014ca7d3', '6ca452a24dbe147205850148d98163481aa22dc6']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['2fa5f435f41242e8ef053e94ae7af400014ca7d3', '6ca452a24dbe147205850148d98163481aa22dc6']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['2a846d2cba5a8f0db089e7f2af275a535b15d82f', 'acaba0aa6a8a55104ae2cb09f093aa30621ffb47']), took the first one with most citations</t>
+          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['2a846d2cba5a8f0db089e7f2af275a535b15d82f', 'acaba0aa6a8a55104ae2cb09f093aa30621ffb47']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I95" t="n">
@@ -3833,7 +3833,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['41f386d38567e38132525cad9bdc7da1ad6e8f1c', '441d6e8ba2cc2314d7d44425a158c25e27f9cb96']), took the first one with most citations</t>
+          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['41f386d38567e38132525cad9bdc7da1ad6e8f1c', '441d6e8ba2cc2314d7d44425a158c25e27f9cb96']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I96" t="n">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['29351b0458efeec9407831afa5be3e3da58f61e1', '7c3b43419293d766b7b6a69c4606d43cbbc13cd2']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['29351b0458efeec9407831afa5be3e3da58f61e1', '7c3b43419293d766b7b6a69c4606d43cbbc13cd2']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I99" t="n">
@@ -3981,7 +3981,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>multiple doi matches ['10123038b80006871abc7396810bed15bfa29387', 'd677e08922a1c646ef739f06bae679cc795ba362'], took the first one with most citations</t>
+          <t>[ss_ids: same DOI] multiple doi matches ['10123038b80006871abc7396810bed15bfa29387', 'd677e08922a1c646ef739f06bae679cc795ba362'], took the first one with most citations</t>
         </is>
       </c>
       <c r="I100" t="n">
@@ -4055,7 +4055,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['32a8259a781ea7255621b0cbdeecfa8d03d7e0bd', 'a7e94f52d1dfb0c5c823032a0b9a70dd0acbb625']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['32a8259a781ea7255621b0cbdeecfa8d03d7e0bd', 'a7e94f52d1dfb0c5c823032a0b9a70dd0acbb625']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I102" t="n">
@@ -4160,7 +4160,7 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['ebb0d21c567909e31be5d43d72c8b3020f2708c9', 'fd2239f855b044b6ebe9fac5e0e01951bc9eddb4']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['ebb0d21c567909e31be5d43d72c8b3020f2708c9', 'fd2239f855b044b6ebe9fac5e0e01951bc9eddb4']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I105" t="n">
@@ -4265,7 +4265,7 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>title matching: single bibkey with multiple_ss_ids (['c52daf1cb971120c4083116cfc213acbaac6faaf', 'cde27a74addf80ca2b3385a32966d51d35e0b2ff']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['c52daf1cb971120c4083116cfc213acbaac6faaf', 'cde27a74addf80ca2b3385a32966d51d35e0b2ff']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I108" t="n">
@@ -4644,6 +4644,99 @@
         <v>2023</v>
       </c>
     </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>1745</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Hend23a</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>article</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Trends in the incidence of pulmonary nodules in chest computed tomography: 10-year results from two Dutch hospitals</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Hendrix, Ward and Rutten, Matthieu and Hendrix, Nils and van Ginneken, Bram and Schaefer-Prokop, Cornelia and Scholten, Ernst T. and Prokop, Mathias and Jacobs, Colin</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr"/>
+      <c r="I121" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>1746</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Graa23a</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>article</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Lumbar spine segmentation in MR images: a dataset and a public benchmark</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>van der Graaf, Jasper W. and van Hooff, Miranda L. and Buckens, Constantinus F. M. and Rutten, Matthieu and van Susante, Job L. C. and Kroeze, Robert Jan and de Kleuver, Marinus and van Ginneken, Bram and Lessmann, Nikolas</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr"/>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr"/>
+      <c r="I122" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>1747</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Thij23</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>article</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Radiomics based automated quality assessment for T2W prostate MR images</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Thijssen, Linda C.P. and de Rooij, Maarten and Barentsz, Jelle O. and Huisman, Henkjan J.</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr"/>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr"/>
+      <c r="I123" t="n">
+        <v>2023</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Renaming and initial file to add SS data to diag.bib
</commit_message>
<xml_diff>
--- a/scripts/script_data/TEMP_LOOKUP_matches_single_bibkey_with_none_one_or_many_ss_ids.xlsx
+++ b/scripts/script_data/TEMP_LOOKUP_matches_single_bibkey_with_none_one_or_many_ss_ids.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,7 +809,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>bc6b483f9b1fa630fa4b43158b13716f1ca7497b</t>
+          <t>4bcd672218ecec70473c84f6f1cc52c64031f3e5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -902,11 +902,11 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bult19</t>
+          <t>Busc16</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -916,40 +916,28 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Epithelium segmentation using deep learning in H\&amp;E-stained prostate specimens with immunohistochemistry as reference standard</t>
+          <t>Risk factors for COPD exacerbations in inhaled medication users: the COPDGene study biannual longitudinal follow-up prospective cohort</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Wouter Bulten and P\'{e}ter B\'{a}ndi and Jeffrey Hoven and Rob {van de Loo} and Johannes Lotz and Nick Weiss and Jeroen {van der Laak} and Bram {van Ginneken} and Christina {Hulsbergen-van de Kaa} and Geert Litjens</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>d5b8fba71671814445de80d36a2d563f43eb9d07</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>['b0cc9473a96dcd45dd1c7de2d7d217c2a453a850', 'd5b8fba71671814445de80d36a2d563f43eb9d07']</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['b0cc9473a96dcd45dd1c7de2d7d217c2a453a850', 'd5b8fba71671814445de80d36a2d563f43eb9d07']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Busch, Robert and Han, MeiLan K and Bowler, Russell P and Dransfield, Mark T and Wells, J Michael and Regan, Elizabeth A and Hersh, Craig P and {COPDGene Investigators</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Busc16</t>
+          <t>Char18</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -959,28 +947,40 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Risk factors for COPD exacerbations in inhaled medication users: the COPDGene study biannual longitudinal follow-up prospective cohort</t>
+          <t>Automatic segmentation of the solid core and enclosed vessels in subsolid pulmonary nodules</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Busch, Robert and Han, MeiLan K and Bowler, Russell P and Dransfield, Mark T and Wells, J Michael and Regan, Elizabeth A and Hersh, Craig P and {COPDGene Investigators</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+          <t>Charbonnier, Jean-Paul and Chung, Kaman and Scholten, Ernst T and van Rikxoort, Eva M and Jacobs, Colin and Sverzellati, Nicola and Silva, Mario and Pastorino, Ugo and van Ginneken, Bram and Ciompi, Francesco</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>3ed451d2830a2afcbbd254f0015eeafa796ba1b7</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>['3ed451d2830a2afcbbd254f0015eeafa796ba1b7', '4fd1ad386d794e9baff286b212013b3b44bb7bd3']</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['3ed451d2830a2afcbbd254f0015eeafa796ba1b7', '4fd1ad386d794e9baff286b212013b3b44bb7bd3']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I14" t="n">
-        <v>2016</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Char18</t>
+          <t>Chle18</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -990,27 +990,27 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Automatic segmentation of the solid core and enclosed vessels in subsolid pulmonary nodules</t>
+          <t>Automatic liver tumor segmentation in {CT} with fully convolutional neural networks and object-based postprocessing</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Charbonnier, Jean-Paul and Chung, Kaman and Scholten, Ernst T and van Rikxoort, Eva M and Jacobs, Colin and Sverzellati, Nicola and Silva, Mario and Pastorino, Ugo and van Ginneken, Bram and Ciompi, Francesco</t>
+          <t>Chlebus, Grzegorz and Schenk, Andrea and Moltz, Jan Hendrik and van Ginneken, Bram and Hahn, Horst Karl and Meine, Hans</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>3ed451d2830a2afcbbd254f0015eeafa796ba1b7</t>
+          <t>27cebb08aca785444166209593fc0ec740469b1b</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['3ed451d2830a2afcbbd254f0015eeafa796ba1b7', '4fd1ad386d794e9baff286b212013b3b44bb7bd3']</t>
+          <t>['27cebb08aca785444166209593fc0ec740469b1b', '96438076b4dfa87956f55c0d8cef9c198de2beb7']</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['3ed451d2830a2afcbbd254f0015eeafa796ba1b7', '4fd1ad386d794e9baff286b212013b3b44bb7bd3']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['27cebb08aca785444166209593fc0ec740469b1b', '96438076b4dfa87956f55c0d8cef9c198de2beb7']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1019,11 +1019,11 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>200</v>
+        <v>232</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Chle18</t>
+          <t>Ciom17a</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1033,40 +1033,40 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Automatic liver tumor segmentation in {CT} with fully convolutional neural networks and object-based postprocessing</t>
+          <t>Towards automatic pulmonary nodule management in lung cancer screening with deep learning</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Chlebus, Grzegorz and Schenk, Andrea and Moltz, Jan Hendrik and van Ginneken, Bram and Hahn, Horst Karl and Meine, Hans</t>
+          <t>F. Ciompi and K. Chung and S. J. van Riel and A. A. A. Setio and P. K. Gerke and C. Jacobs and E. Th. Scholten and C. M. Schaefer-Prokop and M. M. W. Wille and A. Marchiano and U. Pastorino and M. Prokop and B. van Ginneken</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>27cebb08aca785444166209593fc0ec740469b1b</t>
+          <t>fd0901b1f2121506391a7859de8fb695d159a393</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['27cebb08aca785444166209593fc0ec740469b1b', '96438076b4dfa87956f55c0d8cef9c198de2beb7']</t>
+          <t>['86b9d39fb026746752f95f87f87fd26b8512c913', 'fd0901b1f2121506391a7859de8fb695d159a393']</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['27cebb08aca785444166209593fc0ec740469b1b', '96438076b4dfa87956f55c0d8cef9c198de2beb7']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['86b9d39fb026746752f95f87f87fd26b8512c913', 'fd0901b1f2121506391a7859de8fb695d159a393']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ciom17a</t>
+          <t>Dama22</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1076,40 +1076,28 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Towards automatic pulmonary nodule management in lung cancer screening with deep learning</t>
+          <t>A Comparison Between Single- and Multi-Scale Approaches for Classification of Histopathology Images</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>F. Ciompi and K. Chung and S. J. van Riel and A. A. A. Setio and P. K. Gerke and C. Jacobs and E. Th. Scholten and C. M. Schaefer-Prokop and M. M. W. Wille and A. Marchiano and U. Pastorino and M. Prokop and B. van Ginneken</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>fd0901b1f2121506391a7859de8fb695d159a393</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>['86b9d39fb026746752f95f87f87fd26b8512c913', 'fd0901b1f2121506391a7859de8fb695d159a393']</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['86b9d39fb026746752f95f87f87fd26b8512c913', 'fd0901b1f2121506391a7859de8fb695d159a393']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Marina D'Amato and Przemys{\l}aw Szostak and Benjamin Torben-Nielsen</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
-        <v>2017</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>246</v>
+        <v>292</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Dama22</t>
+          <t>Emau15</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1119,145 +1107,145 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>A Comparison Between Single- and Multi-Scale Approaches for Classification of Histopathology Images</t>
+          <t>MR} Imaging as an Additional Screening Modality for the Detection of Breast Cancer in Women Aged 50-75 Years with Extremely Dense Breasts: The {DENSE} Trial Study Design</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Marina D'Amato and Przemys{\l}aw Szostak and Benjamin Torben-Nielsen</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+          <t>Emaus, Marleen J. and Bakker, Marije F. and Peeters, Petra H M. and Loo, Claudette E. and Mann, Ritse M. and {de Jong}, Mathijn D F. and Bisschops, Robertus H C. and Veltman, Jeroen and Duvivier, Katya M. and Lobbes, Marc B I. and Pijnappel, Ruud M. and Karssemeijer, Nico and {de Koning}, Harry J. and {van den Bosch}, Maurice A A J. and Monninkhof, Evelyn M. and Mali, Willem P Th M. and Veldhuis, Wouter B. and {van Gils}, Carla H.</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>fb1084b454e9b6f203c860e6f89ca4389cd1a8e9</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>['fb1084b454e9b6f203c860e6f89ca4389cd1a8e9', 'fc7b70a4d154e3d2dfabe4393809dfb29cc36a7a']</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['fb1084b454e9b6f203c860e6f89ca4389cd1a8e9', 'fc7b70a4d154e3d2dfabe4393809dfb29cc36a7a']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I18" t="n">
-        <v>2022</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Emau15</t>
+          <t>Fary20a</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>MR} Imaging as an Additional Screening Modality for the Detection of Breast Cancer in Women Aged 50-75 Years with Extremely Dense Breasts: The {DENSE} Trial Study Design</t>
+          <t>Attention-guided classification of abnormalities in semi-structured computed tomography reports</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Emaus, Marleen J. and Bakker, Marije F. and Peeters, Petra H M. and Loo, Claudette E. and Mann, Ritse M. and {de Jong}, Mathijn D F. and Bisschops, Robertus H C. and Veltman, Jeroen and Duvivier, Katya M. and Lobbes, Marc B I. and Pijnappel, Ruud M. and Karssemeijer, Nico and {de Koning}, Harry J. and {van den Bosch}, Maurice A A J. and Monninkhof, Evelyn M. and Mali, Willem P Th M. and Veldhuis, Wouter B. and {van Gils}, Carla H.</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>fb1084b454e9b6f203c860e6f89ca4389cd1a8e9</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>['fb1084b454e9b6f203c860e6f89ca4389cd1a8e9', 'fc7b70a4d154e3d2dfabe4393809dfb29cc36a7a']</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['fb1084b454e9b6f203c860e6f89ca4389cd1a8e9', 'fc7b70a4d154e3d2dfabe4393809dfb29cc36a7a']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Khrystyna Faryna and Fakrul I. Tushar and Vincent M. D'Anniballe and Rui Hou and Geoffrey D. Rubin and Joseph Y. Lo</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
-        <v>2015</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>310</v>
+        <v>341</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Fary20a</t>
+          <t>Gall17</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Attention-guided classification of abnormalities in semi-structured computed tomography reports</t>
+          <t>Computed tomography quantification of tracheal abnormalities in {COPD} and their influence on airflow limitation</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Khrystyna Faryna and Fakrul I. Tushar and Vincent M. D'Anniballe and Rui Hou and Geoffrey D. Rubin and Joseph Y. Lo</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+          <t>Gallardo Estrella, Leticia and Pompe, Esther and Kuhnigk, Jan-Martin and Lynch, David A and Bhatt, Surya P and van Ginneken, Bram and van Rikxoort, Eva Marjolein</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>e15e0cd21632aa9d6643b314a4d1d1a6580f2b39</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>['d1e0a041fc417d82c584191ecf5b3b536127d9e0', 'e15e0cd21632aa9d6643b314a4d1d1a6580f2b39']</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['d1e0a041fc417d82c584191ecf5b3b536127d9e0', 'e15e0cd21632aa9d6643b314a4d1d1a6580f2b39']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I20" t="n">
-        <v>2020</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Gall17</t>
+          <t>Garc15</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Computed tomography quantification of tracheal abnormalities in {COPD} and their influence on airflow limitation</t>
+          <t>Comparing regional breast density using {F}ull-{F}ield {D}igital {M}ammograms and {M}agnetic {R}esonance {I}maging: A preliminary study</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Gallardo Estrella, Leticia and Pompe, Esther and Kuhnigk, Jan-Martin and Lynch, David A and Bhatt, Surya P and van Ginneken, Bram and van Rikxoort, Eva Marjolein</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>e15e0cd21632aa9d6643b314a4d1d1a6580f2b39</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>['d1e0a041fc417d82c584191ecf5b3b536127d9e0', 'e15e0cd21632aa9d6643b314a4d1d1a6580f2b39']</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['d1e0a041fc417d82c584191ecf5b3b536127d9e0', 'e15e0cd21632aa9d6643b314a4d1d1a6580f2b39']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Garcia, E. and Oliver, A. and Diez, Y. and Diaz O. and Georgii, J. and Gubern-M\'{e}rida, A. and Mart\'{i}, J. and Mart\'{i}, R.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
-        <v>2017</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Garc15</t>
+          <t>Garc16</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1267,133 +1255,133 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Comparing regional breast density using {F}ull-{F}ield {D}igital {M}ammograms and {M}agnetic {R}esonance {I}maging: A preliminary study</t>
+          <t>Comparison of Four Breast Tissue Segmentation Algorithms for Multi-modal MRI to X-ray Mammography Registration</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Garcia, E. and Oliver, A. and Diez, Y. and Diaz O. and Georgii, J. and Gubern-M\'{e}rida, A. and Mart\'{i}, J. and Mart\'{i}, R.</t>
+          <t>Garc\'{i}a, E. and Oliver, A. and Diez, Y. and Diaz, O. and Gubern-M\'{e}rida, A. and Llad\'{o}, X. and Mart\'{i}, J.</t>
         </is>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Garc16</t>
+          <t>Gees19</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Comparison of Four Breast Tissue Segmentation Algorithms for Multi-modal MRI to X-ray Mammography Registration</t>
+          <t>Computer aided quantification of intratumoral stroma yields an independent prognosticator in rectal cancer</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Garc\'{i}a, E. and Oliver, A. and Diez, Y. and Diaz, O. and Gubern-M\'{e}rida, A. and Llad\'{o}, X. and Mart\'{i}, J.</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+          <t>Geessink, Oscar and Baidoshvili, Alexi and Klaase, Joost and Ehteshami Bejnordi, Babak and Litjens, Geert and van Pelt, Gabi and Mesker, Wilma and Nagtegaal, Iris and Ciompi, Francesco and van der Laak, Jeroen</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>c7ce6b90707871b922aca4cb6a8b16625980788b</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>['2d7797e69a35b5ffe021a2762ef251764562dca4', 'c7ce6b90707871b922aca4cb6a8b16625980788b']</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['2d7797e69a35b5ffe021a2762ef251764562dca4', 'c7ce6b90707871b922aca4cb6a8b16625980788b']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I23" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Gees19</t>
+          <t>Geor16</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Computer aided quantification of intratumoral stroma yields an independent prognosticator in rectal cancer</t>
+          <t>Simulation and Visualization to Support Breast Surgery Planning</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Geessink, Oscar and Baidoshvili, Alexi and Klaase, Joost and Ehteshami Bejnordi, Babak and Litjens, Geert and van Pelt, Gabi and Mesker, Wilma and Nagtegaal, Iris and Ciompi, Francesco and van der Laak, Jeroen</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>c7ce6b90707871b922aca4cb6a8b16625980788b</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>['2d7797e69a35b5ffe021a2762ef251764562dca4', 'c7ce6b90707871b922aca4cb6a8b16625980788b']</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['2d7797e69a35b5ffe021a2762ef251764562dca4', 'c7ce6b90707871b922aca4cb6a8b16625980788b']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Georgii, J. and Paetz, T. and Harz, M. and Stoecker, C. and Rothgang, M. and Colletta, J. and Schilling, K. and Schlooz-Vries, M. and Mann, R.M. and Hahn, H. K.</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Geor16</t>
+          <t>Gern18</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Simulation and Visualization to Support Breast Surgery Planning</t>
+          <t>Automatic quantification of calcifications in the coronary arteries and thoracic aorta on radiotherapy planning {CT} scans of {Western} and {Asian} breast cancer patients</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Georgii, J. and Paetz, T. and Harz, M. and Stoecker, C. and Rothgang, M. and Colletta, J. and Schilling, K. and Schlooz-Vries, M. and Mann, R.M. and Hahn, H. K.</t>
+          <t>Gernaat, Sofie A. M. and van Velzen, Sanne G. M. and Koh, Vicky and Emaus, Marleen J. and I{\v{s}}gum, Ivana and Lessmann, Nikolas and Moes, Shinta and Jacobson, Anouk and Tan, Poey W. and Grobbee, Diederick E. and van den Bongard, Desiree H. J. and Tang, Johann I. and Verkooijen, Helena M.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
-        <v>2016</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Gern18</t>
+          <t>Ghaf17c</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1403,28 +1391,40 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Automatic quantification of calcifications in the coronary arteries and thoracic aorta on radiotherapy planning {CT} scans of {Western} and {Asian} breast cancer patients</t>
+          <t>Location Sensitive Deep Convolutional Neural Networks for Segmentation of White Matter Hyperintensities</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Gernaat, Sofie A. M. and van Velzen, Sanne G. M. and Koh, Vicky and Emaus, Marleen J. and I{\v{s}}gum, Ivana and Lessmann, Nikolas and Moes, Shinta and Jacobson, Anouk and Tan, Poey W. and Grobbee, Diederick E. and van den Bongard, Desiree H. J. and Tang, Johann I. and Verkooijen, Helena M.</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
+          <t>Mohsen Ghafoorian and Nico Karssemeijer and Tom Heskes and Inge van Uden and Clara I. S\'{a}nchez and Geert Litjens and Frank-Erik de Leeuw and Bram van Ginneken and Elena Marchiori and Bram Platel</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>91feb0cb04d67a5c38d0a4e7c67fc7874491abc6</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>['91feb0cb04d67a5c38d0a4e7c67fc7874491abc6', '925024223075dcc5b4db81f4b07eddf2cbdf4519']</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['91feb0cb04d67a5c38d0a4e7c67fc7874491abc6', '925024223075dcc5b4db81f4b07eddf2cbdf4519']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I26" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>367</v>
+        <v>419</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Ghaf17c</t>
+          <t>Ginn17</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1434,27 +1434,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Location Sensitive Deep Convolutional Neural Networks for Segmentation of White Matter Hyperintensities</t>
+          <t>Fifty years of computer analysis in chest imaging: rule-based, machine learning, deep learning</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Mohsen Ghafoorian and Nico Karssemeijer and Tom Heskes and Inge van Uden and Clara I. S\'{a}nchez and Geert Litjens and Frank-Erik de Leeuw and Bram van Ginneken and Elena Marchiori and Bram Platel</t>
+          <t>van Ginneken, Bram</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>91feb0cb04d67a5c38d0a4e7c67fc7874491abc6</t>
+          <t>b69fe5a837277ddbea5215d6bacd3a902e9d11ce</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>['91feb0cb04d67a5c38d0a4e7c67fc7874491abc6', '925024223075dcc5b4db81f4b07eddf2cbdf4519']</t>
+          <t>['46479bbea7749cb2db35b139206039531327053c', 'b69fe5a837277ddbea5215d6bacd3a902e9d11ce']</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['91feb0cb04d67a5c38d0a4e7c67fc7874491abc6', '925024223075dcc5b4db81f4b07eddf2cbdf4519']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['46479bbea7749cb2db35b139206039531327053c', 'b69fe5a837277ddbea5215d6bacd3a902e9d11ce']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -1463,11 +1463,11 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Ginn17</t>
+          <t>Ginn20</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1477,40 +1477,40 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Fifty years of computer analysis in chest imaging: rule-based, machine learning, deep learning</t>
+          <t>The Potential of Artificial Intelligence to Analyze Chest Radiographs for Signs of {COVID}-19 Pneumonia</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>van Ginneken, Bram</t>
+          <t>Bram van Ginneken</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>b69fe5a837277ddbea5215d6bacd3a902e9d11ce</t>
+          <t>11cfab281e93fa7803931be8b589aa1f09d7af02</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>['46479bbea7749cb2db35b139206039531327053c', 'b69fe5a837277ddbea5215d6bacd3a902e9d11ce']</t>
+          <t>['11cfab281e93fa7803931be8b589aa1f09d7af02', '8c4fab5306f4c4e179cfae2acd3427fb5d661627']</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['46479bbea7749cb2db35b139206039531327053c', 'b69fe5a837277ddbea5215d6bacd3a902e9d11ce']), took the first one with most citations</t>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['11cfab281e93fa7803931be8b589aa1f09d7af02', '8c4fab5306f4c4e179cfae2acd3427fb5d661627']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Ginn20</t>
+          <t>Gonz19b</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1520,40 +1520,28 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>The Potential of Artificial Intelligence to Analyze Chest Radiographs for Signs of {COVID}-19 Pneumonia</t>
+          <t>Iterative augmentation of visual evidence for weakly-supervised lesion localization in deep interpretability frameworks</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Bram van Ginneken</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>11cfab281e93fa7803931be8b589aa1f09d7af02</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>['11cfab281e93fa7803931be8b589aa1f09d7af02', '8c4fab5306f4c4e179cfae2acd3427fb5d661627']</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['11cfab281e93fa7803931be8b589aa1f09d7af02', '8c4fab5306f4c4e179cfae2acd3427fb5d661627']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Gonz\'{a}lez-Gonzalo, Cristina and Liefers, Bart and van Ginneken, Bram and S\'{a}nchez, Clara I</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Gonz19b</t>
+          <t>Goud20</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1563,90 +1551,102 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Iterative augmentation of visual evidence for weakly-supervised lesion localization in deep interpretability frameworks</t>
+          <t>Tussen data en theorie</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Gonz\'{a}lez-Gonzalo, Cristina and Liefers, Bart and van Ginneken, Bram and S\'{a}nchez, Clara I</t>
+          <t>Goudsmit, Jeroen and Teuwen, Jonas</t>
         </is>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>443</v>
+        <v>476</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Goud20</t>
+          <t>Gube15d</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Tussen data en theorie</t>
+          <t>Pectoral muscle surface segmentation in automated 3{D} breast ultrasound using cylindrical transform and atlas information</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Goudsmit, Jeroen and Teuwen, Jonas</t>
+          <t>Gubern-M\'{e}rida, A. and Tan, T. and van Zelst, J. and Mann, R. M. and Platel, B. and Karssemeijer, N.</t>
         </is>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Gube15d</t>
+          <t>Habi20</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Pectoral muscle surface segmentation in automated 3{D} breast ultrasound using cylindrical transform and atlas information</t>
+          <t>Evaluation of computer aided detection of tuberculosis on chest radiography among people with diabetes in Karachi Pakistan</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Gubern-M\'{e}rida, A. and Tan, T. and van Zelst, J. and Mann, R. M. and Platel, B. and Karssemeijer, N.</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
+          <t>Habib, Shifa Salman and Rafiq, Sana and Zaidi, Syed Mohammad Asad and Ferrand, Rashida Abbas and Creswell, Jacob and Van Ginneken, Bram and Jamal, Wafa Zehra and Azeemi, Kiran Sohail and Khowaja, Saira and Khan, Aamir</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>13122b7c0ef4a596875eff981651d60140e67417</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>['13122b7c0ef4a596875eff981651d60140e67417', '142f9f46a9ca5a99de4c7b819d801d245a9334ba']</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['13122b7c0ef4a596875eff981651d60140e67417', '142f9f46a9ca5a99de4c7b819d801d245a9334ba']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I32" t="n">
-        <v>2015</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>482</v>
+        <v>500</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Habi20</t>
+          <t>Hayd15a</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1656,40 +1656,28 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Evaluation of computer aided detection of tuberculosis on chest radiography among people with diabetes in Karachi Pakistan</t>
+          <t>Childhood pneumonia increases risk for chronic obstructive pulmonary disease: the COPDGene study</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Habib, Shifa Salman and Rafiq, Sana and Zaidi, Syed Mohammad Asad and Ferrand, Rashida Abbas and Creswell, Jacob and Van Ginneken, Bram and Jamal, Wafa Zehra and Azeemi, Kiran Sohail and Khowaja, Saira and Khan, Aamir</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>13122b7c0ef4a596875eff981651d60140e67417</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>['13122b7c0ef4a596875eff981651d60140e67417', '142f9f46a9ca5a99de4c7b819d801d245a9334ba']</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['13122b7c0ef4a596875eff981651d60140e67417', '142f9f46a9ca5a99de4c7b819d801d245a9334ba']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Hayden, Lystra P. and Hobbs, Brian D. and Cohen, Robyn T. and Wise, Robert A. and Checkley, William and Crapo, James D. and Hersh, Craig P. and {COPDGene Investigators</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
       <c r="I33" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Hayd15a</t>
+          <t>Hayd18</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1699,28 +1687,28 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Childhood pneumonia increases risk for chronic obstructive pulmonary disease: the COPDGene study</t>
+          <t>Childhood asthma is associated with COPD and known asthma variants in COPDGene: a genome-wide association study</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Hayden, Lystra P. and Hobbs, Brian D. and Cohen, Robyn T. and Wise, Robert A. and Checkley, William and Crapo, James D. and Hersh, Craig P. and {COPDGene Investigators</t>
+          <t>Hayden, Lystra P and Cho, Michael H and Raby, Benjamin A and Beaty, Terri H and Silverman, Edwin K and Hersh, Craig P and COPDGene Investigators</t>
         </is>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="n">
-        <v>2015</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Hayd18</t>
+          <t>Hees19</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1730,28 +1718,40 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Childhood asthma is associated with COPD and known asthma variants in COPDGene: a genome-wide association study</t>
+          <t>Genetic risk score has added value over initial clinical grading stage in predicting disease progression in age-related macular degeneration</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Hayden, Lystra P and Cho, Michael H and Raby, Benjamin A and Beaty, Terri H and Silverman, Edwin K and Hersh, Craig P and COPDGene Investigators</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+          <t>Heesterbeek, Thomas J and de Jong, Eiko K and Acar, Ilhan E and Groenewoud, Joannes M M and Liefers, Bart and S\'{a}nchez, Clara I. and Peto, Tunde and Hoyng, Carel B and Pauleikhoff, Daniel and Hense, Hans W and den Hollander, Anneke I</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>560e2100afbc64953c5155459b1f459f6e55003e</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>['560e2100afbc64953c5155459b1f459f6e55003e', '65e6296fe63fbf76519ef01e16b5e62bfabbc3ca']</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['560e2100afbc64953c5155459b1f459f6e55003e', '65e6296fe63fbf76519ef01e16b5e62bfabbc3ca']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I35" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>502</v>
+        <v>523</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Hees19</t>
+          <t>Herm21</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1761,40 +1761,40 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Genetic risk score has added value over initial clinical grading stage in predicting disease progression in age-related macular degeneration</t>
+          <t>Quantitative assessment of inflammatory infiltrates in kidney transplant biopsies using multiplex tyramide signal amplification and deep learning</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Heesterbeek, Thomas J and de Jong, Eiko K and Acar, Ilhan E and Groenewoud, Joannes M M and Liefers, Bart and S\'{a}nchez, Clara I. and Peto, Tunde and Hoyng, Carel B and Pauleikhoff, Daniel and Hense, Hans W and den Hollander, Anneke I</t>
+          <t>Hermsen, Meyke AND Volk, Valery AND Brasen, Jan Hinrich AND Geijs, Daan J AND Gwinner, Wilfried AND Kers, Jesper AND Linmans, Jasper AND Schaadt, Nadine S AND Schmitz, Jessica AND Steenbergen, Eric J AND Swiderska-Chadaj, Zaneta AND Smeets, Bart AND Hilbrands, Luuk L AND van der Laak, Jeroen A W M</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>560e2100afbc64953c5155459b1f459f6e55003e</t>
+          <t>3881ae992914cd50a14782104170cc5dd5d9ae7e</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>['560e2100afbc64953c5155459b1f459f6e55003e', '65e6296fe63fbf76519ef01e16b5e62bfabbc3ca']</t>
+          <t>['3881ae992914cd50a14782104170cc5dd5d9ae7e', 'a4d4e42f1accfd77f378549c776b7c850afbcda5']</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['560e2100afbc64953c5155459b1f459f6e55003e', '65e6296fe63fbf76519ef01e16b5e62bfabbc3ca']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['3881ae992914cd50a14782104170cc5dd5d9ae7e', 'a4d4e42f1accfd77f378549c776b7c850afbcda5']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Herm21</t>
+          <t>Heuv16</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1804,31 +1804,31 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Quantitative assessment of inflammatory infiltrates in kidney transplant biopsies using multiplex tyramide signal amplification and deep learning</t>
+          <t>Automated detection of cerebral microbleeds in patients with Traumatic Brain Injury</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Hermsen, Meyke AND Volk, Valery AND Brasen, Jan Hinrich AND Geijs, Daan J AND Gwinner, Wilfried AND Kers, Jesper AND Linmans, Jasper AND Schaadt, Nadine S AND Schmitz, Jessica AND Steenbergen, Eric J AND Swiderska-Chadaj, Zaneta AND Smeets, Bart AND Hilbrands, Luuk L AND van der Laak, Jeroen A W M</t>
+          <t>Thomas L. A. van den Heuvel and Anke W. van der Eerden and Rashindra Manniesing and Mohsen Ghafoorian and Tao Tan and Teuntje M. J. C. Andriessen and Thijs Vande Vyvere and Luc van den Hauwe and Bart M. ter Haar Romeny and Bozena M. Goraj and Bram Platel</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>3881ae992914cd50a14782104170cc5dd5d9ae7e</t>
+          <t>2e5d61cc075f2a07f75282ae00b2da4a727f5795</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>['3881ae992914cd50a14782104170cc5dd5d9ae7e', 'a4d4e42f1accfd77f378549c776b7c850afbcda5']</t>
+          <t>['2e5d61cc075f2a07f75282ae00b2da4a727f5795', '490b2120bffd758919d924ee1b062789aed16ef3']</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['3881ae992914cd50a14782104170cc5dd5d9ae7e', 'a4d4e42f1accfd77f378549c776b7c850afbcda5']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['2e5d61cc075f2a07f75282ae00b2da4a727f5795', '490b2120bffd758919d924ee1b062789aed16ef3']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="38">
@@ -1907,7 +1907,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -2060,12 +2060,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>['5e3b8647dd6da802cd06a3e8f193d4b2f2823410', 'a908e3775fd064b0d249728a7261cfb1efa13b87']</t>
+          <t>['a908e3775fd064b0d249728a7261cfb1efa13b87', 'b8c484519a8970bf4cb07c3c609c41a05365f258']</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['5e3b8647dd6da802cd06a3e8f193d4b2f2823410', 'a908e3775fd064b0d249728a7261cfb1efa13b87']), took the first one with most citations</t>
+          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['a908e3775fd064b0d249728a7261cfb1efa13b87', 'b8c484519a8970bf4cb07c3c609c41a05365f258']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -2074,11 +2074,11 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Kort15</t>
+          <t>Kos20</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2088,40 +2088,40 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>4D}-{CTA} in Neurovascular Disease: A Review</t>
+          <t>Pitfalls in assessing stromal tumor infiltrating lymphocytes ({sTILs}) in breast cancer</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Hans G. J. Kortman and Ewoud J. Smit and Marcel T. H. Oei and Rashindra Manniesing and Mathias Prokop and Frederick J. A. Meijer</t>
+          <t>Zuzana Kos and and Elvire Roblin and Rim S. Kim and Stefan Michiels and Brandon D. Gallas and Weijie Chen and Koen K. van de Vijver and Shom Goel and Sylvia Adams and Sandra Demaria and Giuseppe Viale and Torsten O. Nielsen and Sunil S. Badve and W. Fraser Symmans and Christos Sotiriou and David L. Rimm and Stephen Hewitt and Carsten Denkert and Sibylle Loibl and Stephen J. Luen and John M. S. Bartlett and Peter Savas and Giancarlo Pruneri and Deborah A. Dillon and Maggie Chon U. Cheang and Andrew Tutt and Jacqueline A. Hall and Marleen Kok and Hugo M. Horlings and Anant Madabhushi and Jeroen van der Laak and Francesco Ciompi and Anne-Vibeke Laenkholm and Enrique Bellolio and Tina Gruosso and Stephen B. Fox and Juan Carlos Araya and Giuseppe Floris and Jan Hude{\v{c}}ek and Leonie Voorwerk and Andrew H. Beck and Jen Kerner and Denis Larsimont and Sabine Declercq and Gert Van den Eynden and Lajos Pusztai and Anna Ehinger and Wentao Yang and Khalid AbdulJabbar and Yinyin Yuan and Rajendra Singh and Crispin Hiley and Maise al Bakir and Alexander J. Lazar and Stephen Naber and Stephan Wienert and Miluska Castillo and Giuseppe Curigliano and Maria-Vittoria Dieci and Fabrice Andr{\'{e}} and Charles Swanton and Jorge Reis-Filho and Joseph Sparano and Eva Balslev and I-Chun Chen and Elisabeth Ida Specht Stovgaard and Katherine Pogue-Geile and Kim R. M. Blenman and Fr{\'{e}}d{\'{e}}rique Penault-Llorca and Stuart Schnitt and Sunil R. Lakhani and Anne Vincent-Salomon and Federico Rojo and Jeremy P. Braybrooke and Matthew G. Hanna and M. Teresa Soler-Mons{\'{o}} and Daniel Bethmann and Carlos A. Castaneda and Karen Willard-Gallo and Ashish Sharma and Huang-Chun Lien and Susan Fineberg and Jeppe Thagaard and Laura Comerma and Paula Gonzalez-Ericsson and Edi Brogi and Sherene Loi and Joel Saltz and Frederick Klaushen and Lee Cooper and Mohamed Amgad and David A. Moore and Roberto Salgado</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>88b86ad75e10c7dac7b70edbd05ed494d699ffb0</t>
+          <t>a7f96553bc690f6f66697895a98e9377cc0f7562</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>['7c83ece3400fa10da80bd363c15dd96eded51c9f', '88b86ad75e10c7dac7b70edbd05ed494d699ffb0']</t>
+          <t>['889cc0565d6e2e844f4db0132c71a612672d2497', 'a7f96553bc690f6f66697895a98e9377cc0f7562']</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['7c83ece3400fa10da80bd363c15dd96eded51c9f', '88b86ad75e10c7dac7b70edbd05ed494d699ffb0']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['889cc0565d6e2e844f4db0132c71a612672d2497', 'a7f96553bc690f6f66697895a98e9377cc0f7562']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>2015</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>755</v>
+        <v>759</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Kos20</t>
+          <t>Kost16</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2131,71 +2131,59 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Pitfalls in assessing stromal tumor infiltrating lymphocytes ({sTILs}) in breast cancer</t>
+          <t>Predicting Lung Volume Reduction after Endobronchial Valve Therapy Is Maximized Using a Combination of Diagnostic Tools</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Zuzana Kos and and Elvire Roblin and Rim S. Kim and Stefan Michiels and Brandon D. Gallas and Weijie Chen and Koen K. van de Vijver and Shom Goel and Sylvia Adams and Sandra Demaria and Giuseppe Viale and Torsten O. Nielsen and Sunil S. Badve and W. Fraser Symmans and Christos Sotiriou and David L. Rimm and Stephen Hewitt and Carsten Denkert and Sibylle Loibl and Stephen J. Luen and John M. S. Bartlett and Peter Savas and Giancarlo Pruneri and Deborah A. Dillon and Maggie Chon U. Cheang and Andrew Tutt and Jacqueline A. Hall and Marleen Kok and Hugo M. Horlings and Anant Madabhushi and Jeroen van der Laak and Francesco Ciompi and Anne-Vibeke Laenkholm and Enrique Bellolio and Tina Gruosso and Stephen B. Fox and Juan Carlos Araya and Giuseppe Floris and Jan Hude{\v{c}}ek and Leonie Voorwerk and Andrew H. Beck and Jen Kerner and Denis Larsimont and Sabine Declercq and Gert Van den Eynden and Lajos Pusztai and Anna Ehinger and Wentao Yang and Khalid AbdulJabbar and Yinyin Yuan and Rajendra Singh and Crispin Hiley and Maise al Bakir and Alexander J. Lazar and Stephen Naber and Stephan Wienert and Miluska Castillo and Giuseppe Curigliano and Maria-Vittoria Dieci and Fabrice Andr{\'{e}} and Charles Swanton and Jorge Reis-Filho and Joseph Sparano and Eva Balslev and I-Chun Chen and Elisabeth Ida Specht Stovgaard and Katherine Pogue-Geile and Kim R. M. Blenman and Fr{\'{e}}d{\'{e}}rique Penault-Llorca and Stuart Schnitt and Sunil R. Lakhani and Anne Vincent-Salomon and Federico Rojo and Jeremy P. Braybrooke and Matthew G. Hanna and M. Teresa Soler-Mons{\'{o}} and Daniel Bethmann and Carlos A. Castaneda and Karen Willard-Gallo and Ashish Sharma and Huang-Chun Lien and Susan Fineberg and Jeppe Thagaard and Laura Comerma and Paula Gonzalez-Ericsson and Edi Brogi and Sherene Loi and Joel Saltz and Frederick Klaushen and Lee Cooper and Mohamed Amgad and David A. Moore and Roberto Salgado</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>a7f96553bc690f6f66697895a98e9377cc0f7562</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>['889cc0565d6e2e844f4db0132c71a612672d2497', 'a7f96553bc690f6f66697895a98e9377cc0f7562']</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['889cc0565d6e2e844f4db0132c71a612672d2497', 'a7f96553bc690f6f66697895a98e9377cc0f7562']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Koster, T David and van Rikxoort, Eva M and Huebner, Ralf-Harto and Doellinger, Felix and Klooster, Karin and Charbonnier, JP. and Radhakrishnan, Sri and Herth, Felix J F and Slebos, Dirk-Jan</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
       <c r="I46" t="n">
-        <v>2020</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>758</v>
+        <v>780</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Kost16</t>
+          <t>Leem15</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Predicting Lung Volume Reduction after Endobronchial Valve Therapy Is Maximized Using a Combination of Diagnostic Tools</t>
+          <t>A novel spherical shell filter for reducing false positives in automatic detection of pulmonary nodules in thoracic {CT} scans</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Koster, T David and van Rikxoort, Eva M and Huebner, Ralf-Harto and Doellinger, Felix and Klooster, Karin and Charbonnier, JP. and Radhakrishnan, Sri and Herth, Felix J F and Slebos, Dirk-Jan</t>
+          <t>Sil van de Leemput and Frank Dorssers and Babak {Ehteshami Bejnordi</t>
         </is>
       </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="n">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Leem15</t>
+          <t>Leem18b</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2205,28 +2193,28 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>A novel spherical shell filter for reducing false positives in automatic detection of pulmonary nodules in thoracic {CT} scans</t>
+          <t>Stacked Bidirectional Convolutional {LSTM}s for {3D} Non-contrast {CT} Reconstruction from Spatiotemporal {4D CT</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Sil van de Leemput and Frank Dorssers and Babak {Ehteshami Bejnordi</t>
+          <t>van de Leemput, S. C. and Prokop, M. and van Ginneken, B. and Manniesing, R.</t>
         </is>
       </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="n">
-        <v>2015</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Leem18b</t>
+          <t>Leem18c</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2236,12 +2224,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Stacked Bidirectional Convolutional {LSTM}s for {3D} Non-contrast {CT} Reconstruction from Spatiotemporal {4D CT</t>
+          <t>Full Volumetric Brain Tissue Segmentation in Non-contrast {CT} using Memory Efficient Convolutional {LSTM}s</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>van de Leemput, S. C. and Prokop, M. and van Ginneken, B. and Manniesing, R.</t>
+          <t>van de Leemput, S. C. and Patel, A. and Manniesing, R.</t>
         </is>
       </c>
       <c r="F49" t="inlineStr"/>
@@ -2253,11 +2241,11 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>783</v>
+        <v>816</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Leem18c</t>
+          <t>Less18a</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2267,12 +2255,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Full Volumetric Brain Tissue Segmentation in Non-contrast {CT} using Memory Efficient Convolutional {LSTM}s</t>
+          <t>Iterative fully convolutional neural networks for automatic vertebra segmentation</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>van de Leemput, S. C. and Patel, A. and Manniesing, R.</t>
+          <t>Nikolas Lessmann and Bram van Ginneken and Pim A. de Jong and Ivana I{\v{s}}gum</t>
         </is>
       </c>
       <c r="F50" t="inlineStr"/>
@@ -2284,42 +2272,42 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>815</v>
+        <v>831</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Less18a</t>
+          <t>Lief19b</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Iterative fully convolutional neural networks for automatic vertebra segmentation</t>
+          <t>A deep learning model for segmentation of geographic atrophy to study its long-term natural history</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Nikolas Lessmann and Bram van Ginneken and Pim A. de Jong and Ivana I{\v{s}}gum</t>
+          <t>Liefers, Bart and Colijn, Johanna M and Gonz\'{a}lez-Gonzalo, Cristina and Verzijden, Timo and Mitchell, Paul and Hoyng, Carel B and van Ginneken, Bram and Klaver, Caroline CW and S\'{a}nchez, Clara I</t>
         </is>
       </c>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>830</v>
+        <v>907</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Lief19b</t>
+          <t>Maie18a</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2329,28 +2317,40 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>A deep learning model for segmentation of geographic atrophy to study its long-term natural history</t>
+          <t>Why rankings of biomedical image analysis competitions should be interpreted with care</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Liefers, Bart and Colijn, Johanna M and Gonz\'{a}lez-Gonzalo, Cristina and Verzijden, Timo and Mitchell, Paul and Hoyng, Carel B and van Ginneken, Bram and Klaver, Caroline CW and S\'{a}nchez, Clara I</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
+          <t>Maier-Hein, Lena and Eisenmann, Matthias and Reinke, Annika and Onogur, Sinan and Stankovic, Marko and Scholz, Patrick and Arbel, Tal and Bogunovic, Hrvoje and Bradley, Andrew P and Carass, Aaron and Feldmann, Carolin and Frangi, Alejandro F and Full, Peter M and van Ginneken, Bram and Hanbury, Allan and Honauer, Katrin and Kozubek, Michal and Landman, Bennett A and Marz, Keno and Maier, Oskar and Maier-Hein, Klaus and Menze, Bjoern H and Muller, Henning and Neher, Peter F and Niessen, Wiro and Rajpoot, Nasir and Sharp, Gregory C and Sirinukunwattana, Korsuk and Speidel, Stefanie and Stock, Christian and Stoyanov, Danail and Taha, Abdel Aziz and van der Sommen, Fons and Wang, Ching-Wei and Weber, Marc-Andre and Zheng, Guoyan and Jannin, Pierre and Kopp-Schneider, Annette</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>91d23b702b9a59bf75c5162c3250017b526c0e69</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>['8678f63d7a648eb4d0f64e50c8ff5a1c53ac128b', '91d23b702b9a59bf75c5162c3250017b526c0e69', 'bed661aebb0ede3c407e044637ce60a6d7ccfe5f', 'fa96430855d805c045335e70c0b60d3acb8c9a79']</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['8678f63d7a648eb4d0f64e50c8ff5a1c53ac128b', '91d23b702b9a59bf75c5162c3250017b526c0e69', 'bed661aebb0ede3c407e044637ce60a6d7ccfe5f', 'fa96430855d805c045335e70c0b60d3acb8c9a79']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I52" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Maie18a</t>
+          <t>Maie19</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2360,40 +2360,28 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Why rankings of biomedical image analysis competitions should be interpreted with care</t>
+          <t>BIAS: Transparent reporting of biomedical image analysis challenges</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Maier-Hein, Lena and Eisenmann, Matthias and Reinke, Annika and Onogur, Sinan and Stankovic, Marko and Scholz, Patrick and Arbel, Tal and Bogunovic, Hrvoje and Bradley, Andrew P and Carass, Aaron and Feldmann, Carolin and Frangi, Alejandro F and Full, Peter M and van Ginneken, Bram and Hanbury, Allan and Honauer, Katrin and Kozubek, Michal and Landman, Bennett A and Marz, Keno and Maier, Oskar and Maier-Hein, Klaus and Menze, Bjoern H and Muller, Henning and Neher, Peter F and Niessen, Wiro and Rajpoot, Nasir and Sharp, Gregory C and Sirinukunwattana, Korsuk and Speidel, Stefanie and Stock, Christian and Stoyanov, Danail and Taha, Abdel Aziz and van der Sommen, Fons and Wang, Ching-Wei and Weber, Marc-Andre and Zheng, Guoyan and Jannin, Pierre and Kopp-Schneider, Annette</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>91d23b702b9a59bf75c5162c3250017b526c0e69</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>['8678f63d7a648eb4d0f64e50c8ff5a1c53ac128b', '91d23b702b9a59bf75c5162c3250017b526c0e69', 'bed661aebb0ede3c407e044637ce60a6d7ccfe5f', 'fa96430855d805c045335e70c0b60d3acb8c9a79']</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['8678f63d7a648eb4d0f64e50c8ff5a1c53ac128b', '91d23b702b9a59bf75c5162c3250017b526c0e69', 'bed661aebb0ede3c407e044637ce60a6d7ccfe5f', 'fa96430855d805c045335e70c0b60d3acb8c9a79']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Maier-Hein, Lena and Reinke, Annika and Kozubek, Michal and L. Martel, Anne and Arbel, Tal and Eisenmann, Matthias and Hanbuary, Allan and Jannin, Pierre and Muller, Henning and Onogur, Sinan and Saez-Rodriguez, Julio and van Ginneken, Bram and Kopp-Schneider, Annette and Landman, Bennett</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
       <c r="I53" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>907</v>
+        <v>937</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Maie19</t>
+          <t>Mann17</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2403,102 +2391,102 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>BIAS: Transparent reporting of biomedical image analysis challenges</t>
+          <t>White Matter and Gray Matter Segmentation in {4D} Computed Tomography</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Maier-Hein, Lena and Reinke, Annika and Kozubek, Michal and L. Martel, Anne and Arbel, Tal and Eisenmann, Matthias and Hanbuary, Allan and Jannin, Pierre and Muller, Henning and Onogur, Sinan and Saez-Rodriguez, Julio and van Ginneken, Bram and Kopp-Schneider, Annette and Landman, Bennett</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
+          <t>Rashindra Manniesing and Marcel T.H. Oei and Luuk J Oostveen and Jaime Melendez and Ewoud J. Smit and Bram Platel and Clara I S\'{a}nchez and Frederick J.A. Meijer and Mathias Prokop and Bram van Ginneken</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>86bab119f07a492350c6cc7bd06ed91c73ee807a</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>['682e8febc5d053766fefe1ee2de5ca2ff39762f2', '7f1eabb6591699816ccd89e7765a66dc54a7175c', '86bab119f07a492350c6cc7bd06ed91c73ee807a', 'e7f15929ff71a5a33af66ece92d707a7be7aebc8']</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['682e8febc5d053766fefe1ee2de5ca2ff39762f2', '7f1eabb6591699816ccd89e7765a66dc54a7175c', '86bab119f07a492350c6cc7bd06ed91c73ee807a', 'e7f15929ff71a5a33af66ece92d707a7be7aebc8']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I54" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>936</v>
+        <v>945</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Mann17</t>
+          <t>Mehr17</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>White Matter and Gray Matter Segmentation in {4D} Computed Tomography</t>
+          <t>Classification of clinical significance of MRI prostate findings using 3D convolutional neural networks</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Rashindra Manniesing and Marcel T.H. Oei and Luuk J Oostveen and Jaime Melendez and Ewoud J. Smit and Bram Platel and Clara I S\'{a}nchez and Frederick J.A. Meijer and Mathias Prokop and Bram van Ginneken</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>86bab119f07a492350c6cc7bd06ed91c73ee807a</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>['682e8febc5d053766fefe1ee2de5ca2ff39762f2', '7f1eabb6591699816ccd89e7765a66dc54a7175c', '86bab119f07a492350c6cc7bd06ed91c73ee807a', 'e7f15929ff71a5a33af66ece92d707a7be7aebc8']</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['682e8febc5d053766fefe1ee2de5ca2ff39762f2', '7f1eabb6591699816ccd89e7765a66dc54a7175c', '86bab119f07a492350c6cc7bd06ed91c73ee807a', 'e7f15929ff71a5a33af66ece92d707a7be7aebc8']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Mehrtash, Alireza and Sedghi, Alireza and Ghafoorian, Mohsen and Taghipour, Mehdi and Tempany, Clare M. and Wells, William M. and Kapur, Tina and Mousavi, Parvin and Abolmaesumi, Purang and Fedorov, Andriy</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
       <c r="I55" t="n">
         <v>2017</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>944</v>
+        <v>950</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Mehr17</t>
+          <t>Meij15c</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Classification of clinical significance of MRI prostate findings using 3D convolutional neural networks</t>
+          <t>Analysis of perfusion {MRI} in stroke: To deconvolve, or not to deconvolve</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Mehrtash, Alireza and Sedghi, Alireza and Ghafoorian, Mohsen and Taghipour, Mehdi and Tempany, Clare M. and Wells, William M. and Kapur, Tina and Mousavi, Parvin and Abolmaesumi, Purang and Fedorov, Andriy</t>
+          <t>Meijs, Midas and Christensen, Soren and Lansberg, Maarten G and Albers, Gregory W and Calamante, Fernando</t>
         </is>
       </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="n">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>949</v>
+        <v>953</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Meij15c</t>
+          <t>Meij17a</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2508,28 +2496,40 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Analysis of perfusion {MRI} in stroke: To deconvolve, or not to deconvolve</t>
+          <t>Robust Segmentation of the Full Cerebral Vasculature in {4D CT} Images of Suspected Stroke Patients</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Meijs, Midas and Christensen, Soren and Lansberg, Maarten G and Albers, Gregory W and Calamante, Fernando</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
+          <t>Midas Meijs and Ajay Patel and Sil van de Leemput and Mathias Prokop and Ewoud J van Dijk and Frank-Erik de Leeuw and Frederick J. A. Meijer and Bram van Ginneken and Rashindra Manniesing</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>fb5c4bf41fd879c9c64028a817db7f7ab6aba429</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>['6119971f513cfa3a9dce2cff139f041f11bcb404', 'fb5c4bf41fd879c9c64028a817db7f7ab6aba429']</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['6119971f513cfa3a9dce2cff139f041f11bcb404', 'fb5c4bf41fd879c9c64028a817db7f7ab6aba429']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I57" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>952</v>
+        <v>1004</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Meij17a</t>
+          <t>Meye20</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2539,40 +2539,28 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Robust Segmentation of the Full Cerebral Vasculature in {4D CT} Images of Suspected Stroke Patients</t>
+          <t>Anisotropic {3D} Multi-Stream {CNN} for Accurate Prostate Segmentation from Multi-Planar {MRI</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Midas Meijs and Ajay Patel and Sil van de Leemput and Mathias Prokop and Ewoud J van Dijk and Frank-Erik de Leeuw and Frederick J. A. Meijer and Bram van Ginneken and Rashindra Manniesing</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>fb5c4bf41fd879c9c64028a817db7f7ab6aba429</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>['6119971f513cfa3a9dce2cff139f041f11bcb404', 'fb5c4bf41fd879c9c64028a817db7f7ab6aba429']</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['6119971f513cfa3a9dce2cff139f041f11bcb404', 'fb5c4bf41fd879c9c64028a817db7f7ab6aba429']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Anneke Meyer and Grzegorz Chlebus and Marko Rak and Daniel Schindele and Martin Schostak and Bram van Ginneken and Andrea Schenk and Hans Meine and Horst K. Hahn and Andreas Schreiber and Christian Hansen</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
       <c r="I58" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Meye20</t>
+          <t>Meye20a</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2599,47 +2587,47 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>1004</v>
+        <v>1019</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Meye20a</t>
+          <t>Moor18a</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Anisotropic {3D} Multi-Stream {CNN} for Accurate Prostate Segmentation from Multi-Planar {MRI</t>
+          <t>Automated soft tissue lesion detection and segmentation in digital mammography using a u-net deep learning network</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Anneke Meyer and Grzegorz Chlebus and Marko Rak and Daniel Schindele and Martin Schostak and Bram van Ginneken and Andrea Schenk and Hans Meine and Horst K. Hahn and Andreas Schreiber and Christian Hansen</t>
+          <t>Timothy de Moor and Alejandro Rodriguez-Ruiz and Ritse Mann and Jonas Teuwen</t>
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="n">
-        <v>2020</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Moor18a</t>
+          <t>Moor2018</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2649,7 +2637,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Timothy de Moor and Alejandro Rodriguez-Ruiz and Ritse Mann and Jonas Teuwen</t>
+          <t>de Moor, Timothy and Rodriguez-Ruiz, Alejandro and Mann, Ritse and Teuwen, Jonas</t>
         </is>
       </c>
       <c r="F61" t="inlineStr"/>
@@ -2661,11 +2649,11 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>1019</v>
+        <v>1030</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Moor2018</t>
+          <t>Mord18a</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2675,12 +2663,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Automated soft tissue lesion detection and segmentation in digital mammography using a u-net deep learning network</t>
+          <t>The importance of early detection of calcifications associated with breast cancer in screening</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>de Moor, Timothy and Rodriguez-Ruiz, Alejandro and Mann, Ritse and Teuwen, Jonas</t>
+          <t>Mordang, J J and Gubern-Merida, A and Bria, A and Tortorella, F and Mann, R M and Broeders, M J M and den Heeten, G J and Karssemeijer, N</t>
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
@@ -2692,7 +2680,7 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -2723,7 +2711,7 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -2766,7 +2754,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -2809,7 +2797,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -2840,7 +2828,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -2871,7 +2859,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -2914,11 +2902,11 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>1145</v>
+        <v>1133</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Poko15</t>
+          <t>Phil15b</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2928,12 +2916,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Reply to Yaalini Shanmugabavan, Stephanie Guillaumier and Hashim U. Ahmed's Letter to the Editor re: Morgan R. Pokorny, Maarten de Rooij, Earl Duncan, et al. Prospective Study of Diagnostic Accuracy Comparing Prostate Cancer Detection by Transrectal Ultrasound-Guided Biopsy Versus Magnetic Resonance ({MR}) Imaging with Subsequent {MR}-guided Biopsy in Men Without Previous Prostate Biopsies. Eur Urol 2014;66:22-9</t>
+          <t>Automated chest-radiography as a triage for {X}pert testing in resource-constrained settings: a prospective study of diagnostic accuracy and costs</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Pokorny, Morgan and Van de Ven, Wendy and Barentsz, Jelle and Thompson, Leslie</t>
+          <t>R.H.H.M. Philipsen and C. I. S\'{a}nchez and P. Maduskar and J. Melendez and L. Peters-Bax and J.G. Peter and R. Dawson and G. Theron and K. Dheda and B. van Ginneken</t>
         </is>
       </c>
       <c r="F69" t="inlineStr"/>
@@ -2945,11 +2933,11 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>1178</v>
+        <v>1146</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Rein21a</t>
+          <t>Poko15</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2959,40 +2947,28 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Common Limitations of Image Processing Metrics: A Picture Story</t>
+          <t>Reply to Yaalini Shanmugabavan, Stephanie Guillaumier and Hashim U. Ahmed's Letter to the Editor re: Morgan R. Pokorny, Maarten de Rooij, Earl Duncan, et al. Prospective Study of Diagnostic Accuracy Comparing Prostate Cancer Detection by Transrectal Ultrasound-Guided Biopsy Versus Magnetic Resonance ({MR}) Imaging with Subsequent {MR}-guided Biopsy in Men Without Previous Prostate Biopsies. Eur Urol 2014;66:22-9</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Annika Reinke and Matthias Eisenmann and Minu D. Tizabi and Carole H. Sudre and Tim Radsch and Michela Antonelli and Tal Arbel and Spyridon Bakas and M. Jorge Cardoso and Veronika Cheplygina and Keyvan Farahani and Ben Glocker and Doreen Heckmann-Notzel and Fabian Isensee and Pierre Jannin and Charles E. Kahn and Jens Kleesiek and Tahsin Kurc and Michal Kozubek and Bennett A. Landman and Geert Litjens and Klaus Maier-Hein and Bjoern Menze and Henning Muller and Jens Petersen and Mauricio Reyes and Nicola Rieke and Bram Stieltjes and Ronald M. Summers and Sotirios A. Tsaftaris and Bram van Ginneken and Annette Kopp-Schneider and Paul Jager and Lena Maier-Hein</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>787ef2981e94e481432cb2a1296903676ec80fa9</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>['6257ee97417d8bead217991caf7c3cd5b439e040', '787ef2981e94e481432cb2a1296903676ec80fa9']</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>[ss_ids: no DOIs!] title matching: single bibkey with multiple_ss_ids (['6257ee97417d8bead217991caf7c3cd5b439e040', '787ef2981e94e481432cb2a1296903676ec80fa9']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Pokorny, Morgan and Van de Ven, Wendy and Barentsz, Jelle and Thompson, Leslie</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
       <c r="I70" t="n">
-        <v>2021</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Ridg15</t>
+          <t>Rein21a</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3002,71 +2978,83 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Differentiating between Subsolid and Solid Pulmonary Nodules at {CT}: Inter- and Intraobserver Agreement between Experienced Thoracic Radiologists</t>
+          <t>Common Limitations of Image Processing Metrics: A Picture Story</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Ridge, Carole A. and Yildirim, Afra and Boiselle, Phillip M. and Franquet, Tomas and Schaefer-Prokop, Cornelia M. and Tack, Denis and Gevenois, Pierre Alain and Bankier, Alexander A.</t>
+          <t>Annika Reinke and Matthias Eisenmann and Minu D. Tizabi and Carole H. Sudre and Tim Radsch and Michela Antonelli and Tal Arbel and Spyridon Bakas and M. Jorge Cardoso and Veronika Cheplygina and Keyvan Farahani and Ben Glocker and Doreen Heckmann-Notzel and Fabian Isensee and Pierre Jannin and Charles E. Kahn and Jens Kleesiek and Tahsin Kurc and Michal Kozubek and Bennett A. Landman and Geert Litjens and Klaus Maier-Hein and Bjoern Menze and Henning Muller and Jens Petersen and Mauricio Reyes and Nicola Rieke and Bram Stieltjes and Ronald M. Summers and Sotirios A. Tsaftaris and Bram van Ginneken and Annette Kopp-Schneider and Paul Jager and Lena Maier-Hein</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>fdf663cc9dda29d55f2e2f44f9876f3b08f854f8</t>
+          <t>787ef2981e94e481432cb2a1296903676ec80fa9</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>['75bc9847c96d8f319f82d1b9ba01b5a396247152', 'a6a2fed1ee525c0d2a35ae6454660eca53ce03fc', 'fdf663cc9dda29d55f2e2f44f9876f3b08f854f8']</t>
+          <t>['6257ee97417d8bead217991caf7c3cd5b439e040', '787ef2981e94e481432cb2a1296903676ec80fa9']</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>[ss_ids: 2 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['75bc9847c96d8f319f82d1b9ba01b5a396247152', 'a6a2fed1ee525c0d2a35ae6454660eca53ce03fc', 'fdf663cc9dda29d55f2e2f44f9876f3b08f854f8']), took the first one with most citations</t>
+          <t>[ss_ids: no DOIs!] title matching: single bibkey with multiple_ss_ids (['6257ee97417d8bead217991caf7c3cd5b439e040', '787ef2981e94e481432cb2a1296903676ec80fa9']), took the first one with most citations</t>
         </is>
       </c>
       <c r="I71" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>1247</v>
+        <v>1182</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Ruh19</t>
+          <t>Ridg15</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Generating CT-scans with 3D Generative Adversarial Networks Using a Supercomputer</t>
+          <t>Differentiating between Subsolid and Solid Pulmonary Nodules at {CT}: Inter- and Intraobserver Agreement between Experienced Thoracic Radiologists</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Ruhe, David and Codreanu, Valeriu and van Leeuwen, Caspar and Podareanu, Damian and Saletore, Vikram and Teuwen, Jonas</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
-      <c r="H72" t="inlineStr"/>
+          <t>Ridge, Carole A. and Yildirim, Afra and Boiselle, Phillip M. and Franquet, Tomas and Schaefer-Prokop, Cornelia M. and Tack, Denis and Gevenois, Pierre Alain and Bankier, Alexander A.</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>fdf663cc9dda29d55f2e2f44f9876f3b08f854f8</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>['75bc9847c96d8f319f82d1b9ba01b5a396247152', 'a6a2fed1ee525c0d2a35ae6454660eca53ce03fc', 'fdf663cc9dda29d55f2e2f44f9876f3b08f854f8']</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>[ss_ids: 2 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['75bc9847c96d8f319f82d1b9ba01b5a396247152', 'a6a2fed1ee525c0d2a35ae6454660eca53ce03fc', 'fdf663cc9dda29d55f2e2f44f9876f3b08f854f8']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I72" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Saha20a</t>
+          <t>Ruh19</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3076,28 +3064,28 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Weakly Supervised 3D Classification of Chest CT using Aggregated Multi-Resolution Deep Segmentation Features</t>
+          <t>Generating CT-scans with 3D Generative Adversarial Networks Using a Supercomputer</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Anindo Saha and Fakrul Tushar and Khrystyna Faryna and Vincent D'Anniballe and Rui Hou and Maciej Mazurowski and Geoffrey Rubin and Joseph Lo</t>
+          <t>Ruhe, David and Codreanu, Valeriu and van Leeuwen, Caspar and Podareanu, Damian and Saletore, Vikram and Teuwen, Jonas</t>
         </is>
       </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Saha20c</t>
+          <t>Saha20a</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3107,12 +3095,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Leveraging Adaptive Color Augmentation in Convolutional Neural Networks for Deep Skin Lesion Segmentation</t>
+          <t>Weakly Supervised 3D Classification of Chest CT using Aggregated Multi-Resolution Deep Segmentation Features</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Anindo Saha and Prem Prasad and Abdullah Thabit</t>
+          <t>Anindo Saha and Fakrul Tushar and Khrystyna Faryna and Vincent D'Anniballe and Rui Hou and Maciej Mazurowski and Geoffrey Rubin and Joseph Lo</t>
         </is>
       </c>
       <c r="F74" t="inlineStr"/>
@@ -3124,11 +3112,11 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>1259</v>
+        <v>1253</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Saha23b</t>
+          <t>Saha20c</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3138,59 +3126,59 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Artificial Intelligence and Radiologists at Prostate Cancer Detection in MRI: The PI-CAI Challenge</t>
+          <t>Leveraging Adaptive Color Augmentation in Convolutional Neural Networks for Deep Skin Lesion Segmentation</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Anindo Saha and Joeran Bosma and Jasper Twilt and Bram van Ginneken and Derya Yakar and Mattijs Elschot and Jeroen Veltman and Jurgen Fütterer and Maarten de Rooij and Henkjan Huisman</t>
+          <t>Anindo Saha and Prem Prasad and Abdullah Thabit</t>
         </is>
       </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="n">
-        <v>2023</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>1326</v>
+        <v>1260</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Scha20</t>
+          <t>Saha23b</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Model-based Prediction of Critical Illness in Hospitalized Patients with COVID-19</t>
+          <t>Artificial Intelligence and Radiologists at Prostate Cancer Detection in MRI: The PI-CAI Challenge</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Schalekamp, S and Huisman, M and van Dijk, R A and Boomsma, M F and Freire Jorge, P J and de Boer, W S and Herder, G J M and Bonarius, M and Groot, O A and Jong, E and Schreuder, A and Schaefer-Prokop, C M</t>
+          <t>Anindo Saha and Joeran Bosma and Jasper Twilt and Bram van Ginneken and Derya Yakar and Mattijs Elschot and Jeroen Veltman and Jurgen Fütterer and Maarten de Rooij and Henkjan Huisman</t>
         </is>
       </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="n">
-        <v>2020</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Scha22a</t>
+          <t>Scha20</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3200,28 +3188,28 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Current and emerging artificial intelligence applications in chest imaging: a pediatric perspective</t>
+          <t>Model-based Prediction of Critical Illness in Hospitalized Patients with COVID-19</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Schalekamp, Steven and Klein, Willemijn M and van Leeuwen, Kicky G</t>
+          <t>Schalekamp, S and Huisman, M and van Dijk, R A and Boomsma, M F and Freire Jorge, P J and de Boer, W S and Herder, G J M and Bonarius, M and Groot, O A and Jong, E and Schreuder, A and Schaefer-Prokop, C M</t>
         </is>
       </c>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="n">
-        <v>2022</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>1364</v>
+        <v>1329</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Scho14c</t>
+          <t>Scha22a</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3231,40 +3219,28 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Towards a close computed tomography monitoring approach for screen detected subsolid pulmonary nodules?</t>
+          <t>Current and emerging artificial intelligence applications in chest imaging: a pediatric perspective</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Scholten, Ernst T. and de Jong, Pim A. and de Hoop, Bartjan and van Klaveren, Rob and van Amelsvoort-van de Vorst, Saskia and Oudkerk, Matthijs and Vliegenthart, Rozemarijn and de Koning, Harry J. and van der Aalst, Carlijn M. and Vernhout, Ren\'{e} M. and Groen, Harry J M. and Lammers, Jan-Willem J. and van Ginneken, Bram and Jacobs, Colin and Mali, Willem P T M. and Horeweg, Nanda and Weenink, Carla and Thunnissen, Erik and Prokop, Mathias and Gietema, Hester A.</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>6ca452a24dbe147205850148d98163481aa22dc6</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>['2fa5f435f41242e8ef053e94ae7af400014ca7d3', '6ca452a24dbe147205850148d98163481aa22dc6']</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['2fa5f435f41242e8ef053e94ae7af400014ca7d3', '6ca452a24dbe147205850148d98163481aa22dc6']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Schalekamp, Steven and Klein, Willemijn M and van Leeuwen, Kicky G</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr"/>
       <c r="I78" t="n">
-        <v>2015</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Scho15b</t>
+          <t>Scho14c</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3274,28 +3250,40 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Computed tomographic characteristics of interval and post screen carcinomas in lung cancer screening</t>
+          <t>Towards a close computed tomography monitoring approach for screen detected subsolid pulmonary nodules?</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Scholten, Ernst Th and Horeweg, Nanda and {de Koning}, Harry J. and Vliegenthart, Rozemarijn and Oudkerk, Matthijs and Mali, Willem P Th M. and {de Jong}, Pim A.</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr"/>
-      <c r="G79" t="inlineStr"/>
-      <c r="H79" t="inlineStr"/>
+          <t>Scholten, Ernst T. and de Jong, Pim A. and de Hoop, Bartjan and van Klaveren, Rob and van Amelsvoort-van de Vorst, Saskia and Oudkerk, Matthijs and Vliegenthart, Rozemarijn and de Koning, Harry J. and van der Aalst, Carlijn M. and Vernhout, Ren\'{e} M. and Groen, Harry J M. and Lammers, Jan-Willem J. and van Ginneken, Bram and Jacobs, Colin and Mali, Willem P T M. and Horeweg, Nanda and Weenink, Carla and Thunnissen, Erik and Prokop, Mathias and Gietema, Hester A.</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>6ca452a24dbe147205850148d98163481aa22dc6</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>['2fa5f435f41242e8ef053e94ae7af400014ca7d3', '6ca452a24dbe147205850148d98163481aa22dc6']</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['2fa5f435f41242e8ef053e94ae7af400014ca7d3', '6ca452a24dbe147205850148d98163481aa22dc6']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I79" t="n">
         <v>2015</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>1379</v>
+        <v>1369</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Schr19a</t>
+          <t>Scho15b</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3305,50 +3293,50 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Morphological and topographical appearance of microaneurysms on optical coherence tomography angiography</t>
+          <t>Computed tomographic characteristics of interval and post screen carcinomas in lung cancer screening</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Schreur, Vivian and Domanian, Artin and Liefers, Bart and Venhuizen, Freerk G. and Klevering, B. Jeroen and Hoyng, Carel B. and de Jong, Eiko K. and Theelen, Thomas</t>
+          <t>Scholten, Ernst Th and Horeweg, Nanda and {de Koning}, Harry J. and Vliegenthart, Rozemarijn and Oudkerk, Matthijs and Mali, Willem P Th M. and {de Jong}, Pim A.</t>
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
       <c r="I80" t="n">
-        <v>2019</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>1393</v>
+        <v>1380</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Schw15</t>
+          <t>Schr19a</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Automatic assessment of nipple position in {A}utomated 3{D} {B}reast {U}ltrasound images</t>
+          <t>Morphological and topographical appearance of microaneurysms on optical coherence tomography angiography</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Schwaab, J. and Gubern-M\'{e}rida, A. and Wang, L. and Gunther, M.</t>
+          <t>Schreur, Vivian and Domanian, Artin and Liefers, Bart and Venhuizen, Freerk G. and Klevering, B. Jeroen and Hoyng, Carel B. and de Jong, Eiko K. and Theelen, Thomas</t>
         </is>
       </c>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="82">
@@ -3357,38 +3345,38 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Schw16</t>
+          <t>Schw15</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Automated quality assessment in three-dimensional breast ultrasound images</t>
+          <t>Automatic assessment of nipple position in {A}utomated 3{D} {B}reast {U}ltrasound images</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Schwaab, Julia and Diez, Yago and Oliver, Arnau and Marti, Robert and van Zelst, Jan and Gubern-Merida, Albert and Mourri, Ahmed Bensouda and Gregori, Johannes and Gunther, Matthias</t>
+          <t>Schwaab, J. and Gubern-M\'{e}rida, A. and Wang, L. and Gunther, M.</t>
         </is>
       </c>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="n">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>1408</v>
+        <v>1395</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Sier20</t>
+          <t>Schw16</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3398,28 +3386,28 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Rapid study assessment in follow-up whole-body computed tomography in patients with multiple myeloma using a dedicated bone subtraction software</t>
+          <t>Automated quality assessment in three-dimensional breast ultrasound images</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>M. M. Sieren and F. Brenne and A. Hering and H. Kienapfel and N. Gebauer and T. H. Oechtering and A. F\"{u}rschke and F. Wegner and E. Stahlberg and S. Heldmann and J. Barkhausen and A. Frydrychowicz</t>
+          <t>Schwaab, Julia and Diez, Yago and Oliver, Arnau and Marti, Robert and van Zelst, Jan and Gubern-Merida, Albert and Mourri, Ahmed Bensouda and Gregori, Johannes and Gunther, Matthias</t>
         </is>
       </c>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="n">
-        <v>2020</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>1417</v>
+        <v>1409</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Sleb15</t>
+          <t>Sier20</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3429,81 +3417,81 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Air Trapping in Emphysema</t>
+          <t>Rapid study assessment in follow-up whole-body computed tomography in patients with multiple myeloma using a dedicated bone subtraction software</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Slebos, Dirk-Jan and van Rikxoort, Eva M. and van der Bij, Wim</t>
+          <t>M. M. Sieren and F. Brenne and A. Hering and H. Kienapfel and N. Gebauer and T. H. Oechtering and A. F\"{u}rschke and F. Wegner and E. Stahlberg and S. Heldmann and J. Barkhausen and A. Frydrychowicz</t>
         </is>
       </c>
       <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
       <c r="I84" t="n">
-        <v>2015</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>1435</v>
+        <v>1418</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Smit21</t>
+          <t>Sleb15</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Quality control of whole-slide images through multi-class semantic segmentation of artifacts</t>
+          <t>Air Trapping in Emphysema</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Smit, Gijs and Ciompi, Francesco and Cig{\'e}hn, Maria and Bod{\'e}n, Anna and van der Laak, Jeroen and Mercan, Caner</t>
+          <t>Slebos, Dirk-Jan and van Rikxoort, Eva M. and van der Bij, Wim</t>
         </is>
       </c>
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
       <c r="I85" t="n">
-        <v>2021</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>1447</v>
+        <v>1436</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Spre18</t>
+          <t>Smit21</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Impact of automatically detected motion artifacts on coronary calcium scoring in chest computed tomography</t>
+          <t>Quality control of whole-slide images through multi-class semantic segmentation of artifacts</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Sprem, Jurica and de Vos, Bob D. and Lessmann, Nikolas and de Jong, Pim A. and Viergever, Max A. and Isgum, Ivana</t>
+          <t>Smit, Gijs and Ciompi, Francesco and Cig{\'e}hn, Maria and Bod{\'e}n, Anna and van der Laak, Jeroen and Mercan, Caner</t>
         </is>
       </c>
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr"/>
       <c r="I86" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="87">
@@ -3512,7 +3500,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Spre18a</t>
+          <t>Spre18</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3522,12 +3510,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Coronary calcium scoring with partial volume correction in anthropomorphic thorax phantom and screening chest {CT} images</t>
+          <t>Impact of automatically detected motion artifacts on coronary calcium scoring in chest computed tomography</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Sprem, Jurica and de Vos, Bob D. and Lessmann, Nikolas and van Hamersvelt, Robbert W. and Greuter, Marcel J. W. and de Jong, Pim A. and Leiner, Tim and Viergever, Max A. and Isgum, Ivana</t>
+          <t>Sprem, Jurica and de Vos, Bob D. and Lessmann, Nikolas and de Jong, Pim A. and Viergever, Max A. and Isgum, Ivana</t>
         </is>
       </c>
       <c r="F87" t="inlineStr"/>
@@ -3539,64 +3527,64 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>1479</v>
+        <v>1449</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Stud22</t>
+          <t>Spre18a</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Building-T-cell score is a potential predictor for more aggressive treatment in pT1 colorectal cancers</t>
+          <t>Coronary calcium scoring with partial volume correction in anthropomorphic thorax phantom and screening chest {CT} images</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Linda Studer and John-Melle Bokhorst and Francesco Ciompi and Andreas Fischer and Heather Dawson</t>
+          <t>Sprem, Jurica and de Vos, Bob D. and Lessmann, Nikolas and van Hamersvelt, Robbert W. and Greuter, Marcel J. W. and de Jong, Pim A. and Leiner, Tim and Viergever, Max A. and Isgum, Ivana</t>
         </is>
       </c>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr"/>
       <c r="I88" t="n">
-        <v>2022</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>1514</v>
+        <v>1480</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Teus15</t>
+          <t>Stud22</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Impact of motion-associated noise on intrinsic optical signal imaging in humans with optical coherence tomography</t>
+          <t>Building-T-cell score is a potential predictor for more aggressive treatment in pT1 colorectal cancers</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Michel M. Teussink and Barry Cense and Mark J. J. P. van Grinsven and B. Jeroen Klevering and Carel B. Hoyng and Thomas Theelen</t>
+          <t>Linda Studer and John-Melle Bokhorst and Francesco Ciompi and Andreas Fischer and Heather Dawson</t>
         </is>
       </c>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr"/>
       <c r="I89" t="n">
-        <v>2015</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="90">
@@ -3605,7 +3593,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Teus15a</t>
+          <t>Teus15</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3615,12 +3603,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>OCT Angiography Compared to Fluorescein and Indocyanine Green Angiography in Chronic Central Serous Chorioretinopathy</t>
+          <t>Impact of motion-associated noise on intrinsic optical signal imaging in humans with optical coherence tomography</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Teussink, Michel M. and Breukink, Myrte B. and van Grinsven, Mark J J P. and Hoyng, Carel B. and Klevering, B Jeroen and Boon, Camiel J F. and de Jong, Eiko K. and Theelen, Thomas</t>
+          <t>Michel M. Teussink and Barry Cense and Mark J. J. P. van Grinsven and B. Jeroen Klevering and Carel B. Hoyng and Thomas Theelen</t>
         </is>
       </c>
       <c r="F90" t="inlineStr"/>
@@ -3636,7 +3624,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Teuw14</t>
+          <t>Teus15a</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3646,12 +3634,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>A note on Gaussian maximal function</t>
+          <t>OCT Angiography Compared to Fluorescein and Indocyanine Green Angiography in Chronic Central Serous Chorioretinopathy</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Teuwen, J.</t>
+          <t>Teussink, Michel M. and Breukink, Myrte B. and van Grinsven, Mark J J P. and Hoyng, Carel B. and Klevering, B Jeroen and Boon, Camiel J F. and de Jong, Eiko K. and Theelen, Thomas</t>
         </is>
       </c>
       <c r="F91" t="inlineStr"/>
@@ -3663,11 +3651,11 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Teuw16b</t>
+          <t>Teuw14</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3677,7 +3665,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>On the integral kernels of derivatives of the Ornstein-Uhlenbeck semigroup</t>
+          <t>A note on Gaussian maximal function</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3689,16 +3677,16 @@
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="inlineStr"/>
       <c r="I92" t="n">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>1553</v>
+        <v>1519</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Vele21</t>
+          <t>Teuw16b</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3708,102 +3696,90 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Volumetric evaluation of CT images of adrenal glands in primary aldosteronism.</t>
+          <t>On the integral kernels of derivatives of the Ornstein-Uhlenbeck semigroup</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Velema, M S and Canu, L and Dekkers, T and Hermus, A R M M and Timmers, H J L M and Schultze Kool, L J and Groenewoud, H J M M and Jacobs, C and Deinum, J and SPARTACUS Investigators</t>
+          <t>Teuwen, J.</t>
         </is>
       </c>
       <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>1565</v>
+        <v>1554</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Velz19</t>
+          <t>Vele21</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Direct prediction of cardiovascular mortality from low-dose chest {CT} using deep learning</t>
+          <t>Volumetric evaluation of CT images of adrenal glands in primary aldosteronism.</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Sanne van Velzen and Majd Zreik and Nikolas Lessmann and Max A. Viergever and Pim A. de Jong and Helena M. Verkooijen and Ivana I{\v{s}}gum</t>
+          <t>Velema, M S and Canu, L and Dekkers, T and Hermus, A R M M and Timmers, H J L M and Schultze Kool, L J and Groenewoud, H J M M and Jacobs, C and Deinum, J and SPARTACUS Investigators</t>
         </is>
       </c>
       <c r="F94" t="inlineStr"/>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr"/>
       <c r="I94" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>1581</v>
+        <v>1566</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Vend18</t>
+          <t>Velz19</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Elastic versus rigid image registration in {MRI-TRUS} fusion prostate biopsy: a systematic review and meta-analysis</t>
+          <t>Direct prediction of cardiovascular mortality from low-dose chest {CT} using deep learning</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Venderink, Wulphert and de Rooij, Maarten and Sedelaar, Michiel J. and Huisman, Henkjan J. and Futterer, Jurgen J.</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>acaba0aa6a8a55104ae2cb09f093aa30621ffb47</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>['2a846d2cba5a8f0db089e7f2af275a535b15d82f', 'acaba0aa6a8a55104ae2cb09f093aa30621ffb47']</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['2a846d2cba5a8f0db089e7f2af275a535b15d82f', 'acaba0aa6a8a55104ae2cb09f093aa30621ffb47']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Sanne van Velzen and Majd Zreik and Nikolas Lessmann and Max A. Viergever and Pim A. de Jong and Helena M. Verkooijen and Ivana I{\v{s}}gum</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr"/>
       <c r="I95" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>1597</v>
+        <v>1580</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Vent21</t>
+          <t>Ven16f</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3813,71 +3789,71 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Automated COVID-19 Grading with Convolutional Neural Networks in Computed Tomography Scans: A Systematic Comparison</t>
+          <t>MR}-targeted {TRUS} prostate biopsy using local reference augmentation: initial experience</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Coen de Vente and Luuk H. Boulogne and Kiran Vaidhya Venkadesh and Cheryl Sital and Nikolas Lessmann and Colin Jacobs and Clara I. S\'{a}nchez and Bram van Ginneken</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>441d6e8ba2cc2314d7d44425a158c25e27f9cb96</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>['41f386d38567e38132525cad9bdc7da1ad6e8f1c', '441d6e8ba2cc2314d7d44425a158c25e27f9cb96']</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['41f386d38567e38132525cad9bdc7da1ad6e8f1c', '441d6e8ba2cc2314d7d44425a158c25e27f9cb96']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>van de Ven}, Wendy J. M. and Venderink, Wulphert and Sedelaar, J. P. Michiel and Veltman, Jeroen and Barentsz, Jelle O. and F{\"{u}}tterer, Jurgen J. and Cornel, Erik B. and Huisman, Henkjan J.</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr"/>
       <c r="I96" t="n">
-        <v>2022</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>1600</v>
+        <v>1582</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Verm21</t>
+          <t>Vend18</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>muPEN: Multi-class PseudoEdgeNet for PD-L1 assessment</t>
+          <t>Elastic versus rigid image registration in {MRI-TRUS} fusion prostate biopsy: a systematic review and meta-analysis</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Vermazeren, Jeroen and van Eekelen, Leander and Meesters, Luca and Looijen-Salamon, Monika and Vos, Shoko and Munari, Enrico and Mercan, Caner and Ciompi, Francesco</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr"/>
-      <c r="H97" t="inlineStr"/>
+          <t>Venderink, Wulphert and de Rooij, Maarten and Sedelaar, Michiel J. and Huisman, Henkjan J. and Futterer, Jurgen J.</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>acaba0aa6a8a55104ae2cb09f093aa30621ffb47</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>['2a846d2cba5a8f0db089e7f2af275a535b15d82f', 'acaba0aa6a8a55104ae2cb09f093aa30621ffb47']</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['2a846d2cba5a8f0db089e7f2af275a535b15d82f', 'acaba0aa6a8a55104ae2cb09f093aa30621ffb47']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I97" t="n">
-        <v>2021</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>1619</v>
+        <v>1598</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Vos15</t>
+          <t>Vent21</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3887,71 +3863,71 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Multiparametric Magnetic Resonance Imaging for Discriminating Low-Grade From High-Grade Prostate Cancer</t>
+          <t>Automated COVID-19 Grading with Convolutional Neural Networks in Computed Tomography Scans: A Systematic Comparison</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Vos, Eline K. and Kobus, Thiele and Litjens, Geert J S. and Hambrock, Thomas and Hulsbergen-van de Kaa, Christina A. and Barentsz, Jelle O. and Maas, Marnix C. and Scheenen, Tom W J.</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="inlineStr"/>
-      <c r="H98" t="inlineStr"/>
+          <t>Coen de Vente and Luuk H. Boulogne and Kiran Vaidhya Venkadesh and Cheryl Sital and Nikolas Lessmann and Colin Jacobs and Clara I. S\'{a}nchez and Bram van Ginneken</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>441d6e8ba2cc2314d7d44425a158c25e27f9cb96</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>['41f386d38567e38132525cad9bdc7da1ad6e8f1c', '441d6e8ba2cc2314d7d44425a158c25e27f9cb96']</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['41f386d38567e38132525cad9bdc7da1ad6e8f1c', '441d6e8ba2cc2314d7d44425a158c25e27f9cb96']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I98" t="n">
-        <v>2015</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>1633</v>
+        <v>1601</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Vree18c</t>
+          <t>Verm21</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>The added value of mammography in different age-groups of women with and without BRCA mutation screened with breast MRI</t>
+          <t>muPEN: Multi-class PseudoEdgeNet for PD-L1 assessment</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Vreemann, Suzan and van Zelst, Jan C M and Schlooz-Vries, Margrethe and Bult, Peter and Hoogerbrugge, Nicoline and Karssemeijer, Nico and Gubern-Merida, Albert and Mann, Ritse M</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>7c3b43419293d766b7b6a69c4606d43cbbc13cd2</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>['29351b0458efeec9407831afa5be3e3da58f61e1', '7c3b43419293d766b7b6a69c4606d43cbbc13cd2']</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['29351b0458efeec9407831afa5be3e3da58f61e1', '7c3b43419293d766b7b6a69c4606d43cbbc13cd2']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Vermazeren, Jeroen and van Eekelen, Leander and Meesters, Luca and Looijen-Salamon, Monika and Vos, Shoko and Munari, Enrico and Mercan, Caner and Ciompi, Francesco</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
       <c r="I99" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>1652</v>
+        <v>1620</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Wand17a</t>
+          <t>Vos15</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3961,71 +3937,71 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>The effect of volumetric breast density on the risk of screen-detected and interval breast cancers: a cohort study</t>
+          <t>Multiparametric Magnetic Resonance Imaging for Discriminating Low-Grade From High-Grade Prostate Cancer</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Wanders, Johanna O.P. and Holland, Katharina and Karssemeijer, Nico and Peeters, Petra H.M. and Veldhuis, Wouter B. and Mann, Ritse M. and {van Gils}, Carla H.</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>d677e08922a1c646ef739f06bae679cc795ba362</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>['10123038b80006871abc7396810bed15bfa29387', 'd677e08922a1c646ef739f06bae679cc795ba362']</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>[ss_ids: same DOI] multiple doi matches ['10123038b80006871abc7396810bed15bfa29387', 'd677e08922a1c646ef739f06bae679cc795ba362'], took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Vos, Eline K. and Kobus, Thiele and Litjens, Geert J S. and Hambrock, Thomas and Hulsbergen-van de Kaa, Christina A. and Barentsz, Jelle O. and Maas, Marnix C. and Scheenen, Tom W J.</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
       <c r="I100" t="n">
-        <v>2017</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>1654</v>
+        <v>1634</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Wang15</t>
+          <t>Vree18c</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>A fast alignment method for breast {MRI} follow-up studies using automated breast segmentation and current-prior registration</t>
+          <t>The added value of mammography in different age-groups of women with and without BRCA mutation screened with breast MRI</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Lei Wang and Jan Strehlow and Jan Ruehaak and Florian Weiler and Yago Diez and Albert Gubern-M\'{e}rida and Susanne Diekmann and Hendrik Laue and Horst K. Hahn</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr"/>
-      <c r="G101" t="inlineStr"/>
-      <c r="H101" t="inlineStr"/>
+          <t>Vreemann, Suzan and van Zelst, Jan C M and Schlooz-Vries, Margrethe and Bult, Peter and Hoogerbrugge, Nicoline and Karssemeijer, Nico and Gubern-Merida, Albert and Mann, Ritse M</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>7c3b43419293d766b7b6a69c4606d43cbbc13cd2</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>['29351b0458efeec9407831afa5be3e3da58f61e1', '7c3b43419293d766b7b6a69c4606d43cbbc13cd2']</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['29351b0458efeec9407831afa5be3e3da58f61e1', '7c3b43419293d766b7b6a69c4606d43cbbc13cd2']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I101" t="n">
-        <v>2015</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>1669</v>
+        <v>1653</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Xie20</t>
+          <t>Wand17a</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -4035,71 +4011,71 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Relational Modeling for Robust and Efficient Pulmonary Lobe Segmentation in {CT} Scans</t>
+          <t>The effect of volumetric breast density on the risk of screen-detected and interval breast cancers: a cohort study</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Xie, Weiyi and Jacobs, Colin and Charbonnier, Jean-Paul and van Ginneken, Bram</t>
+          <t>Wanders, Johanna O.P. and Holland, Katharina and Karssemeijer, Nico and Peeters, Petra H.M. and Veldhuis, Wouter B. and Mann, Ritse M. and {van Gils}, Carla H.</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>32a8259a781ea7255621b0cbdeecfa8d03d7e0bd</t>
+          <t>d677e08922a1c646ef739f06bae679cc795ba362</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>['32a8259a781ea7255621b0cbdeecfa8d03d7e0bd', 'a7e94f52d1dfb0c5c823032a0b9a70dd0acbb625']</t>
+          <t>['10123038b80006871abc7396810bed15bfa29387', 'd677e08922a1c646ef739f06bae679cc795ba362']</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>[ss_ids: multiple DOIs!] title matching: single bibkey with multiple_ss_ids (['32a8259a781ea7255621b0cbdeecfa8d03d7e0bd', 'a7e94f52d1dfb0c5c823032a0b9a70dd0acbb625']), took the first one with most citations</t>
+          <t>[ss_ids: same DOI] multiple doi matches ['10123038b80006871abc7396810bed15bfa29387', 'd677e08922a1c646ef739f06bae679cc795ba362'], took the first one with most citations</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>2020</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>1671</v>
+        <v>1655</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Xie21a</t>
+          <t>Wang15</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Dense regression activation maps for lesion segmentation in {CT} scans of {COVID-19} patients</t>
+          <t>A fast alignment method for breast {MRI} follow-up studies using automated breast segmentation and current-prior registration</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Xie, Weiyi and Jacobs, Colin and van Ginneken, Bram</t>
+          <t>Lei Wang and Jan Strehlow and Jan Ruehaak and Florian Weiler and Yago Diez and Albert Gubern-M\'{e}rida and Susanne Diekmann and Hendrik Laue and Horst K. Hahn</t>
         </is>
       </c>
       <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
       <c r="I103" t="n">
-        <v>2021</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>1676</v>
+        <v>1670</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Yous17</t>
+          <t>Xie20</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -4109,28 +4085,40 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Risk stratification based on screening history: the NELSON lung cancer screening study</t>
+          <t>Relational Modeling for Robust and Efficient Pulmonary Lobe Segmentation in {CT} Scans</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Yousaf-Khan, Uraujh and van der Aalst, Carlijn and de Jong, Pim A and Heuvelmans, Marjolein and Scholten, Ernst and Walter, Joan and Nackaerts, Kristiaan and Groen, Harry and Vliegenthart, Rozemarijn and Ten Haaf, Kevin and Oudkerk, Matthijs and de Koning, Harry</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr"/>
-      <c r="G104" t="inlineStr"/>
-      <c r="H104" t="inlineStr"/>
+          <t>Xie, Weiyi and Jacobs, Colin and Charbonnier, Jean-Paul and van Ginneken, Bram</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>32a8259a781ea7255621b0cbdeecfa8d03d7e0bd</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>['32a8259a781ea7255621b0cbdeecfa8d03d7e0bd', 'a114f0f6dbeb11d47d0736a1ece21cbf4be27fb5']</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>[ss_ids: 1 no DOI, rest same DOI] title matching: single bibkey with multiple_ss_ids (['32a8259a781ea7255621b0cbdeecfa8d03d7e0bd', 'a114f0f6dbeb11d47d0736a1ece21cbf4be27fb5']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I104" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>1679</v>
+        <v>1672</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Zaid18</t>
+          <t>Xie21a</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -4140,40 +4128,28 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Evaluation of the diagnostic accuracy of Computer-Aided Detection of tuberculosis on Chest radiography among private sector patients in {P}akistan</t>
+          <t>Dense regression activation maps for lesion segmentation in {CT} scans of {COVID-19} patients</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Zaidi, Syed Mohammad Asad and Habib, Shifa Salman and van Ginneken, Bram and Ferrand, Rashida Abbas and Creswell, Jacob and Khowaja, Saira and Khan, Aamir</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>ebb0d21c567909e31be5d43d72c8b3020f2708c9</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>['ebb0d21c567909e31be5d43d72c8b3020f2708c9', 'fd2239f855b044b6ebe9fac5e0e01951bc9eddb4']</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['ebb0d21c567909e31be5d43d72c8b3020f2708c9', 'fd2239f855b044b6ebe9fac5e0e01951bc9eddb4']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>Xie, Weiyi and Jacobs, Colin and van Ginneken, Bram</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr"/>
       <c r="I105" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>1688</v>
+        <v>1677</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Zels18b</t>
+          <t>Yous17</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -4183,28 +4159,28 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Automated Three-dimensional Breast {US} for Screening: Technique, Artifacts, and Lesion Characterization</t>
+          <t>Risk stratification based on screening history: the NELSON lung cancer screening study</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>van Zelst, Jan C M and Mann, Ritse M</t>
+          <t>Yousaf-Khan, Uraujh and van der Aalst, Carlijn and de Jong, Pim A and Heuvelmans, Marjolein and Scholten, Ernst and Walter, Joan and Nackaerts, Kristiaan and Groen, Harry and Vliegenthart, Rozemarijn and Ten Haaf, Kevin and Oudkerk, Matthijs and de Koning, Harry</t>
         </is>
       </c>
       <c r="F106" t="inlineStr"/>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="inlineStr"/>
       <c r="I106" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>1693</v>
+        <v>1680</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Zrei18</t>
+          <t>Zaid18</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -4214,28 +4190,40 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Deep learning analysis of the myocardium in coronary {CT} angiography for identification of patients with functionally significant coronary artery stenosis</t>
+          <t>Evaluation of the diagnostic accuracy of Computer-Aided Detection of tuberculosis on Chest radiography among private sector patients in {P}akistan</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Majd Zreik and Nikolas Lessmann and Robbert W. van Hamersvelt and Jelmer M. Wolterink and Michiel Voskuil and Max A. Viergever and Tim Leiner and Ivana I{\v{s}}gum</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr"/>
-      <c r="G107" t="inlineStr"/>
-      <c r="H107" t="inlineStr"/>
+          <t>Zaidi, Syed Mohammad Asad and Habib, Shifa Salman and van Ginneken, Bram and Ferrand, Rashida Abbas and Creswell, Jacob and Khowaja, Saira and Khan, Aamir</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>ebb0d21c567909e31be5d43d72c8b3020f2708c9</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>['ebb0d21c567909e31be5d43d72c8b3020f2708c9', 'fd2239f855b044b6ebe9fac5e0e01951bc9eddb4']</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['ebb0d21c567909e31be5d43d72c8b3020f2708c9', 'fd2239f855b044b6ebe9fac5e0e01951bc9eddb4']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I107" t="n">
         <v>2018</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>1705</v>
+        <v>1689</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Hude20</t>
+          <t>Zels18b</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -4245,40 +4233,28 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Application of a risk-management framework for integration of stromal tumor-infiltrating lymphocytes in clinical trials.</t>
+          <t>Automated Three-dimensional Breast {US} for Screening: Technique, Artifacts, and Lesion Characterization</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Hudeček, Jan and Voorwerk, Leonie and van Seijen, Maartje and Nederlof, Iris and de Maaker, Michiel and van den Berg, Jose and van de Vijver, Koen K. and Sikorska, Karolina and Adams, Sylvia and Demaria, Sandra and Viale, Giuseppe and Nielsen, Torsten O. and Badve, Sunil S. and Michiels, Stefan and Symmans, William Fraser and Sotiriou, Christos and Rimm, David L. and Hewitt, Stephen M. and Denkert, Carsten and Loibl, Sibylle and Loi, Sherene and Bartlett, John M. S. and Pruneri, Giancarlo and Dillon, Deborah A. and Cheang, Maggie C. U. and Tutt, Andrew and Hall, Jacqueline A. and Kos, Zuzana and Salgado, Roberto and Kok, Marleen and Horlings, Hugo M. and Group, International Immuno-Oncology Biomarker Working</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>c52daf1cb971120c4083116cfc213acbaac6faaf</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>['c52daf1cb971120c4083116cfc213acbaac6faaf', 'cde27a74addf80ca2b3385a32966d51d35e0b2ff']</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['c52daf1cb971120c4083116cfc213acbaac6faaf', 'cde27a74addf80ca2b3385a32966d51d35e0b2ff']), took the first one with most citations</t>
-        </is>
-      </c>
+          <t>van Zelst, Jan C M and Mann, Ritse M</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr"/>
       <c r="I108" t="n">
-        <v>2020</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>1708</v>
+        <v>1694</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Bohn22</t>
+          <t>Zrei18</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -4288,28 +4264,28 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Digital Implant Planning in Patients with Ectodermal Dysplasia: Clinical Report.</t>
+          <t>Deep learning analysis of the myocardium in coronary {CT} angiography for identification of patients with functionally significant coronary artery stenosis</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Bohner, Lauren and Vinayahalingam, Shankeeth and Kleinheinz, Johannes and Hanisch, Marcel</t>
+          <t>Majd Zreik and Nikolas Lessmann and Robbert W. van Hamersvelt and Jelmer M. Wolterink and Michiel Voskuil and Max A. Viergever and Tim Leiner and Ivana I{\v{s}}gum</t>
         </is>
       </c>
       <c r="F109" t="inlineStr"/>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="inlineStr"/>
       <c r="I109" t="n">
-        <v>2022</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>1709</v>
+        <v>1706</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Naik22</t>
+          <t>Hude20</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -4319,28 +4295,40 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Transforming healthcare through a digital revolution: A review of digital healthcare technologies and solutions.</t>
+          <t>Application of a risk-management framework for integration of stromal tumor-infiltrating lymphocytes in clinical trials.</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Naik, Nithesh and Hameed, B. M. Zeeshan and Sooriyaperakasam, Nilakshman and Vinayahalingam, Shankeeth and Patil, Vathsala and Smriti, Komal and Saxena, Janhavi and Shah, Milap and Ibrahim, Sufyan and Singh, Anshuman and Karimi, Hadis and Naganathan, Karthickeyan and Shetty, Dasharathraj K. and Rai, Bhavan Prasad and Chlosta, Piotr and Somani, Bhaskar K.</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr"/>
-      <c r="G110" t="inlineStr"/>
-      <c r="H110" t="inlineStr"/>
+          <t>Hudeček, Jan and Voorwerk, Leonie and van Seijen, Maartje and Nederlof, Iris and de Maaker, Michiel and van den Berg, Jose and van de Vijver, Koen K. and Sikorska, Karolina and Adams, Sylvia and Demaria, Sandra and Viale, Giuseppe and Nielsen, Torsten O. and Badve, Sunil S. and Michiels, Stefan and Symmans, William Fraser and Sotiriou, Christos and Rimm, David L. and Hewitt, Stephen M. and Denkert, Carsten and Loibl, Sibylle and Loi, Sherene and Bartlett, John M. S. and Pruneri, Giancarlo and Dillon, Deborah A. and Cheang, Maggie C. U. and Tutt, Andrew and Hall, Jacqueline A. and Kos, Zuzana and Salgado, Roberto and Kok, Marleen and Horlings, Hugo M. and Group, International Immuno-Oncology Biomarker Working</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>c52daf1cb971120c4083116cfc213acbaac6faaf</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>['c52daf1cb971120c4083116cfc213acbaac6faaf', 'cde27a74addf80ca2b3385a32966d51d35e0b2ff']</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>[ss_ids: same DOI] title matching: single bibkey with multiple_ss_ids (['c52daf1cb971120c4083116cfc213acbaac6faaf', 'cde27a74addf80ca2b3385a32966d51d35e0b2ff']), took the first one with most citations</t>
+        </is>
+      </c>
       <c r="I110" t="n">
-        <v>2022</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>1712</v>
+        <v>1709</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Bemp22</t>
+          <t>Bohn22</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -4350,12 +4338,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>The role of muscular traction in the occurrence of skeletal relapse after advancement bilateral sagittal split osteotomy (BSSO): A systematic review.</t>
+          <t>Digital Implant Planning in Patients with Ectodermal Dysplasia: Clinical Report.</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Van den Bempt, Maxim and Vinayahalingam, Shankeeth and Han, Michael D. and Bergé, Stefaan J. and Xi, Tong</t>
+          <t>Bohner, Lauren and Vinayahalingam, Shankeeth and Kleinheinz, Johannes and Hanisch, Marcel</t>
         </is>
       </c>
       <c r="F111" t="inlineStr"/>
@@ -4367,11 +4355,11 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>1713</v>
+        <v>1710</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Fehe22</t>
+          <t>Naik22</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4381,12 +4369,12 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Emulating Clinical Diagnostic Reasoning for Jaw Cysts with Machine Learning.</t>
+          <t>Transforming healthcare through a digital revolution: A review of digital healthcare technologies and solutions.</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Feher, Balazs and Kuchler, Ulrike and Schwendicke, Falk and Schneider, Lisa and Cejudo Grano de Oro, Jose Eduardo and Xi, Tong and Vinayahalingam, Shankeeth and Hsu, Tzu-Ming Harry and Brinz, Janet and Chaurasia, Akhilanand and Dhingra, Kunaal and Gaudin, Robert Andre and Mohammad-Rahimi, Hossein and Pereira, Nielsen and Perez-Pastor, Francesc and Tryfonos, Olga and Uribe, Sergio E. and Hanisch, Marcel and Krois, Joachim</t>
+          <t>Naik, Nithesh and Hameed, B. M. Zeeshan and Sooriyaperakasam, Nilakshman and Vinayahalingam, Shankeeth and Patil, Vathsala and Smriti, Komal and Saxena, Janhavi and Shah, Milap and Ibrahim, Sufyan and Singh, Anshuman and Karimi, Hadis and Naganathan, Karthickeyan and Shetty, Dasharathraj K. and Rai, Bhavan Prasad and Chlosta, Piotr and Somani, Bhaskar K.</t>
         </is>
       </c>
       <c r="F112" t="inlineStr"/>
@@ -4398,11 +4386,11 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Esch22</t>
+          <t>Bemp22</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4412,12 +4400,12 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>A Survey on the Use of Artificial Intelligence by Clinicians in Dentistry and Oral and Maxillofacial Surgery.</t>
+          <t>The role of muscular traction in the occurrence of skeletal relapse after advancement bilateral sagittal split osteotomy (BSSO): A systematic review.</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Eschert, Tim and Schwendicke, Falk and Krois, Joachim and Bohner, Lauren and Vinayahalingam, Shankeeth and Hanisch, Marcel</t>
+          <t>Van den Bempt, Maxim and Vinayahalingam, Shankeeth and Han, Michael D. and Bergé, Stefaan J. and Xi, Tong</t>
         </is>
       </c>
       <c r="F113" t="inlineStr"/>
@@ -4429,11 +4417,11 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Chen22</t>
+          <t>Fehe22</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4443,12 +4431,12 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Is the pattern of mandibular asymmetry in mild craniofacial microsomia comparable to non-syndromic class II asymmetry?</t>
+          <t>Emulating Clinical Diagnostic Reasoning for Jaw Cysts with Machine Learning.</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Chen, Yun-Fang and Vinayahalingam, Shankeeth and Bergé, Stefaan and Liao, Yu-Fang and Maal, Thomas and Xi, Tong</t>
+          <t>Feher, Balazs and Kuchler, Ulrike and Schwendicke, Falk and Schneider, Lisa and Cejudo Grano de Oro, Jose Eduardo and Xi, Tong and Vinayahalingam, Shankeeth and Hsu, Tzu-Ming Harry and Brinz, Janet and Chaurasia, Akhilanand and Dhingra, Kunaal and Gaudin, Robert Andre and Mohammad-Rahimi, Hossein and Pereira, Nielsen and Perez-Pastor, Francesc and Tryfonos, Olga and Uribe, Sergio E. and Hanisch, Marcel and Krois, Joachim</t>
         </is>
       </c>
       <c r="F114" t="inlineStr"/>
@@ -4460,11 +4448,11 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Sadr23</t>
+          <t>Esch22</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4474,28 +4462,28 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Deep Learning for Detection of Periapical Radiolucent Lesions: A Systematic Review and Meta-analysis of Diagnostic Test Accuracy.</t>
+          <t>A Survey on the Use of Artificial Intelligence by Clinicians in Dentistry and Oral and Maxillofacial Surgery.</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Sadr, Soroush and Mohammad-Rahimi, Hossein and Motamedian, Saeed Reza and Zahedrozegar, Samira and Motie, Parisa and Vinayahalingam, Shankeeth and Dianat, Omid and Nosrat, Ali</t>
+          <t>Eschert, Tim and Schwendicke, Falk and Krois, Joachim and Bohner, Lauren and Vinayahalingam, Shankeeth and Hanisch, Marcel</t>
         </is>
       </c>
       <c r="F115" t="inlineStr"/>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
       <c r="I115" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>1720</v>
+        <v>1716</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Graa23</t>
+          <t>Chen22</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -4505,74 +4493,74 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>MRI image features with an evident relation to low back pain: a narrative review</t>
+          <t>Is the pattern of mandibular asymmetry in mild craniofacial microsomia comparable to non-syndromic class II asymmetry?</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>van der Graaf, Jasper W and Kroeze, Robert Jan and Buckens, Constantinus FM and Lessmann, Nikolas and van Hooff, Miranda L</t>
+          <t>Chen, Yun-Fang and Vinayahalingam, Shankeeth and Bergé, Stefaan and Liao, Yu-Fang and Maal, Thomas and Xi, Tong</t>
         </is>
       </c>
       <c r="F116" t="inlineStr"/>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr"/>
       <c r="I116" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>1722</v>
+        <v>1718</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Alves22c</t>
+          <t>Sadr23</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Uncertainty-Guided Self-learning Framework for Semi-supervised Multi-organ Segmentation</t>
+          <t>Deep Learning for Detection of Periapical Radiolucent Lesions: A Systematic Review and Meta-analysis of Diagnostic Test Accuracy.</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Alves, Nat{\'a}lia and de Wilde, Bram</t>
+          <t>Sadr, Soroush and Mohammad-Rahimi, Hossein and Motamedian, Saeed Reza and Zahedrozegar, Samira and Motie, Parisa and Vinayahalingam, Shankeeth and Dianat, Omid and Nosrat, Ali</t>
         </is>
       </c>
       <c r="F117" t="inlineStr"/>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr"/>
       <c r="I117" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>1725</v>
+        <v>1721</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Bosma23a</t>
+          <t>Graa23</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>inproceedings</t>
+          <t>article</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Reproducibility of Training Deep Learning Models for Medical Image Analysis</t>
+          <t>MRI image features with an evident relation to low back pain: a narrative review</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Joeran Bosma and Dr{\'e} Peeters and Nat{\'a}lia Alves and Anindo Saha and Zaigham Saghir and Colin Jacobs and Henkjan Huisman</t>
+          <t>van der Graaf, Jasper W and Kroeze, Robert Jan and Buckens, Constantinus FM and Lessmann, Nikolas and van Hooff, Miranda L</t>
         </is>
       </c>
       <c r="F118" t="inlineStr"/>
@@ -4584,11 +4572,11 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>1732</v>
+        <v>1723</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Spro23</t>
+          <t>Alves22c</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4598,28 +4586,28 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>nnUNet meets pathology: bridging the gap for application to whole-slide images and computational biomarkers</t>
+          <t>Uncertainty-Guided Self-learning Framework for Semi-supervised Multi-organ Segmentation</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Joey Spronck and Thijs Gelton and Leander van Eekelen and Joep Bogaerts and Leslie Tessier and Mart van Rijthoven and Lieke van der Woude and Michel van den Heuvel and Willemijn Theelen and Jeroen van der Laak and Francesco Ciompi</t>
+          <t>Alves, Nat{\'a}lia and de Wilde, Bram</t>
         </is>
       </c>
       <c r="F119" t="inlineStr"/>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr"/>
       <c r="I119" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>1740</v>
+        <v>1726</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Vend23</t>
+          <t>Bosma23a</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4629,12 +4617,12 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Automatic quantification of {TSR} as a prognostic marker for pancreatic cancer.</t>
+          <t>Reproducibility of Training Deep Learning Models for Medical Image Analysis</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Vendittelli, Pierpaolo and Bokhorst, John-Melle and Smeets, Esther Markus and Kryklyva, Valentyna and Brosens, Lodewijk and Verbeke, Caroline and Litjens, Geert</t>
+          <t>Joeran Bosma and Dr{\'e} Peeters and Nat{\'a}lia Alves and Anindo Saha and Zaigham Saghir and Colin Jacobs and Henkjan Huisman</t>
         </is>
       </c>
       <c r="F120" t="inlineStr"/>
@@ -4646,26 +4634,26 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>1745</v>
+        <v>1733</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Hend23a</t>
+          <t>Spro23</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Trends in the incidence of pulmonary nodules in chest computed tomography: 10-year results from two Dutch hospitals</t>
+          <t>nnUNet meets pathology: bridging the gap for application to whole-slide images and computational biomarkers</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Hendrix, Ward and Rutten, Matthieu and Hendrix, Nils and van Ginneken, Bram and Schaefer-Prokop, Cornelia and Scholten, Ernst T. and Prokop, Mathias and Jacobs, Colin</t>
+          <t>Joey Spronck and Thijs Gelton and Leander van Eekelen and Joep Bogaerts and Leslie Tessier and Mart van Rijthoven and Lieke van der Woude and Michel van den Heuvel and Willemijn Theelen and Jeroen van der Laak and Francesco Ciompi</t>
         </is>
       </c>
       <c r="F121" t="inlineStr"/>
@@ -4677,26 +4665,26 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>1746</v>
+        <v>1741</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Graa23a</t>
+          <t>Vend23</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>article</t>
+          <t>inproceedings</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Lumbar spine segmentation in MR images: a dataset and a public benchmark</t>
+          <t>Automatic quantification of {TSR} as a prognostic marker for pancreatic cancer.</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>van der Graaf, Jasper W. and van Hooff, Miranda L. and Buckens, Constantinus F. M. and Rutten, Matthieu and van Susante, Job L. C. and Kroeze, Robert Jan and de Kleuver, Marinus and van Ginneken, Bram and Lessmann, Nikolas</t>
+          <t>Vendittelli, Pierpaolo and Bokhorst, John-Melle and Smeets, Esther Markus and Kryklyva, Valentyna and Brosens, Lodewijk and Verbeke, Caroline and Litjens, Geert</t>
         </is>
       </c>
       <c r="F122" t="inlineStr"/>
@@ -4706,37 +4694,6 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>1747</v>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>Thij23</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>article</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>Radiomics based automated quality assessment for T2W prostate MR images</t>
-        </is>
-      </c>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>Thijssen, Linda C.P. and de Rooij, Maarten and Barentsz, Jelle O. and Huisman, Henkjan J.</t>
-        </is>
-      </c>
-      <c r="F123" t="inlineStr"/>
-      <c r="G123" t="inlineStr"/>
-      <c r="H123" t="inlineStr"/>
-      <c r="I123" t="n">
-        <v>2023</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>